<commit_message>
Update news for v4.14 (#1080)
</commit_message>
<xml_diff>
--- a/src/main/webapp/content/files/oncologyTherapies/fda_approved_oncology_therapies.xlsx
+++ b/src/main/webapp/content/files/oncologyTherapies/fda_approved_oncology_therapies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhangh2/repos/oncokb-public/src/main/webapp/content/files/precisionOncologyTherapies/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luc2\Desktop\oncokb\oncokb-public\src\main\webapp\content\files\oncologyTherapies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B72AEB6C-18D0-6F4C-83BC-96CFF5054C45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F379A9-3BA0-4568-815E-3A57B2186A86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20200" xr2:uid="{D862B214-800F-AF40-9BAA-60FE1781D5C8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{D862B214-800F-AF40-9BAA-60FE1781D5C8}"/>
   </bookViews>
   <sheets>
     <sheet name="FDA-Approved Oncology Therapies" sheetId="1" r:id="rId1"/>
@@ -1439,9 +1439,6 @@
   </si>
   <si>
     <t>PIK3CA, AKT1 or PTEN Oncogenic Mutations and HR+/HER2-</t>
-  </si>
-  <si>
-    <t>FGFR2 Fusions,FGFR3 Fusions, S249C, R248C, G370C, Y373C</t>
   </si>
   <si>
     <r>
@@ -1683,6 +1680,9 @@
   </si>
   <si>
     <t>Abbreviations: NGS: Next-generation sequencing, ER: Estrogen receptor, HR: Hormone receptor, MSI-H: Microsatellite instability-high, HRR: Homologous recombination repair, TMB-H: Tumor mutational burden-high, dMMR: Mismatch repair deficient, pMMR: Mismatch repair proficient, PSMA: Prostate-specific membrane antigen, ITD: Internal tandem duplication, TKD: Tyrosine kinase domain, Ph+: Philadelphia chromosome +</t>
+  </si>
+  <si>
+    <t>FGFR3-TACC3 Fusion, FGFR3-BAIAP2L1 Fusion, FGFR3 S249C, R248C, G370C, Y373C</t>
   </si>
 </sst>
 </file>
@@ -2113,32 +2113,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B89377A-76F6-CA40-8081-AAD80BFAB6B8}">
   <dimension ref="A1:H218"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="149" zoomScaleNormal="150" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A143" zoomScale="149" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D147" sqref="D147"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.5" customWidth="1"/>
-    <col min="2" max="2" width="22.1640625" customWidth="1"/>
-    <col min="3" max="3" width="26.1640625" customWidth="1"/>
-    <col min="4" max="4" width="25.83203125" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" customWidth="1"/>
+    <col min="2" max="2" width="22.19921875" customWidth="1"/>
+    <col min="3" max="3" width="26.19921875" customWidth="1"/>
+    <col min="4" max="4" width="25.796875" customWidth="1"/>
+    <col min="5" max="5" width="27.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>461</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>462</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>463</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>464</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>1</v>
@@ -2147,10 +2149,10 @@
         <v>2</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -2173,7 +2175,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
@@ -2196,7 +2198,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -2222,7 +2224,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
@@ -2245,7 +2247,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
@@ -2268,7 +2270,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>3</v>
       </c>
@@ -2294,7 +2296,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>3</v>
       </c>
@@ -2317,7 +2319,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>3</v>
       </c>
@@ -2343,7 +2345,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>3</v>
       </c>
@@ -2369,7 +2371,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="5" customFormat="1" ht="70" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:8" s="5" customFormat="1" ht="66" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>3</v>
       </c>
@@ -2395,7 +2397,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>3</v>
       </c>
@@ -2418,7 +2420,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>3</v>
       </c>
@@ -2441,7 +2443,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>3</v>
       </c>
@@ -2467,7 +2469,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>3</v>
       </c>
@@ -2490,7 +2492,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>3</v>
       </c>
@@ -2513,7 +2515,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>2002</v>
       </c>
@@ -2539,7 +2541,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>2002</v>
       </c>
@@ -2562,7 +2564,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>2002</v>
       </c>
@@ -2585,7 +2587,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>2003</v>
       </c>
@@ -2609,7 +2611,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>2003</v>
       </c>
@@ -2632,7 +2634,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>2003</v>
       </c>
@@ -2658,7 +2660,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>2003</v>
       </c>
@@ -2684,7 +2686,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>2004</v>
       </c>
@@ -2707,7 +2709,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>2004</v>
       </c>
@@ -2730,7 +2732,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:8" s="5" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:8" s="5" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>2004</v>
       </c>
@@ -2756,7 +2758,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>2004</v>
       </c>
@@ -2779,7 +2781,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>2004</v>
       </c>
@@ -2805,7 +2807,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>2004</v>
       </c>
@@ -2829,7 +2831,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>2005</v>
       </c>
@@ -2852,7 +2854,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>2005</v>
       </c>
@@ -2875,7 +2877,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>2006</v>
       </c>
@@ -2901,7 +2903,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>2006</v>
       </c>
@@ -2924,7 +2926,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>2006</v>
       </c>
@@ -2947,7 +2949,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:8" s="5" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:8" s="5" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>2006</v>
       </c>
@@ -2973,7 +2975,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>2006</v>
       </c>
@@ -2999,7 +3001,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>2006</v>
       </c>
@@ -3022,7 +3024,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>2007</v>
       </c>
@@ -3046,7 +3048,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>2007</v>
       </c>
@@ -3072,7 +3074,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>2007</v>
       </c>
@@ -3098,7 +3100,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>2007</v>
       </c>
@@ -3122,7 +3124,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>2008</v>
       </c>
@@ -3145,7 +3147,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>2008</v>
       </c>
@@ -3168,7 +3170,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:8" s="5" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>2009</v>
       </c>
@@ -3194,7 +3196,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>2009</v>
       </c>
@@ -3217,7 +3219,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>2009</v>
       </c>
@@ -3240,7 +3242,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>2009</v>
       </c>
@@ -3264,7 +3266,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>2009</v>
       </c>
@@ -3287,7 +3289,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>2010</v>
       </c>
@@ -3310,7 +3312,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>2010</v>
       </c>
@@ -3334,7 +3336,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>2010</v>
       </c>
@@ -3357,7 +3359,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>2011</v>
       </c>
@@ -3380,7 +3382,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <v>2011</v>
       </c>
@@ -3404,7 +3406,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>2011</v>
       </c>
@@ -3430,7 +3432,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>2011</v>
       </c>
@@ -3456,7 +3458,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
         <v>2011</v>
       </c>
@@ -3480,7 +3482,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <v>2011</v>
       </c>
@@ -3503,7 +3505,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <v>2011</v>
       </c>
@@ -3526,7 +3528,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <v>2011</v>
       </c>
@@ -3550,7 +3552,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <v>2011</v>
       </c>
@@ -3576,7 +3578,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
         <v>2012</v>
       </c>
@@ -3599,7 +3601,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
         <v>2012</v>
       </c>
@@ -3623,7 +3625,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A63" s="5">
         <v>2012</v>
       </c>
@@ -3649,7 +3651,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A64" s="5">
         <v>2012</v>
       </c>
@@ -3672,7 +3674,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A65" s="5">
         <v>2012</v>
       </c>
@@ -3696,7 +3698,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A66" s="5">
         <v>2012</v>
       </c>
@@ -3719,7 +3721,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A67" s="5">
         <v>2012</v>
       </c>
@@ -3742,7 +3744,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A68" s="5">
         <v>2012</v>
       </c>
@@ -3768,7 +3770,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A69" s="5">
         <v>2012</v>
       </c>
@@ -3794,7 +3796,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A70" s="5">
         <v>2012</v>
       </c>
@@ -3820,7 +3822,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A71" s="5">
         <v>2012</v>
       </c>
@@ -3844,7 +3846,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A72" s="5">
         <v>2013</v>
       </c>
@@ -3870,7 +3872,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A73" s="5">
         <v>2013</v>
       </c>
@@ -3896,7 +3898,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A74" s="5">
         <v>2013</v>
       </c>
@@ -3922,7 +3924,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A75" s="5">
         <v>2013</v>
       </c>
@@ -3948,7 +3950,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A76" s="5">
         <v>2013</v>
       </c>
@@ -3971,7 +3973,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="77" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A77" s="5">
         <v>2013</v>
       </c>
@@ -3995,7 +3997,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A78" s="5">
         <v>2013</v>
       </c>
@@ -4018,7 +4020,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="79" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A79" s="5">
         <v>2013</v>
       </c>
@@ -4044,7 +4046,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A80" s="5">
         <v>2014</v>
       </c>
@@ -4068,7 +4070,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="81" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A81" s="5">
         <v>2014</v>
       </c>
@@ -4094,7 +4096,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="82" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A82" s="5">
         <v>2014</v>
       </c>
@@ -4120,7 +4122,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A83" s="5">
         <v>2014</v>
       </c>
@@ -4146,7 +4148,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A84" s="5">
         <v>2014</v>
       </c>
@@ -4169,7 +4171,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A85" s="5">
         <v>2014</v>
       </c>
@@ -4192,7 +4194,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="86" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A86" s="5">
         <v>2014</v>
       </c>
@@ -4216,7 +4218,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="87" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A87" s="5">
         <v>2014</v>
       </c>
@@ -4242,7 +4244,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="88" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A88" s="5">
         <v>2014</v>
       </c>
@@ -4268,7 +4270,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="89" spans="1:8" s="5" customFormat="1" ht="56" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:8" s="5" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A89" s="5">
         <v>2014</v>
       </c>
@@ -4294,7 +4296,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="90" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A90" s="5">
         <v>2014</v>
       </c>
@@ -4317,7 +4319,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="91" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A91" s="5">
         <v>2014</v>
       </c>
@@ -4340,7 +4342,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A92" s="5">
         <v>2015</v>
       </c>
@@ -4366,7 +4368,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="93" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A93" s="5">
         <v>2015</v>
       </c>
@@ -4392,7 +4394,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="94" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A94" s="5">
         <v>2015</v>
       </c>
@@ -4415,7 +4417,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A95" s="5">
         <v>2015</v>
       </c>
@@ -4439,7 +4441,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A96" s="5">
         <v>2015</v>
       </c>
@@ -4462,7 +4464,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A97" s="5">
         <v>2015</v>
       </c>
@@ -4488,7 +4490,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="98" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A98" s="5">
         <v>2015</v>
       </c>
@@ -4512,7 +4514,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A99" s="5">
         <v>2015</v>
       </c>
@@ -4535,7 +4537,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A100" s="5">
         <v>2015</v>
       </c>
@@ -4558,7 +4560,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="1:8" s="5" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:8" s="5" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A101" s="5">
         <v>2015</v>
       </c>
@@ -4584,7 +4586,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="102" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A102" s="5">
         <v>2015</v>
       </c>
@@ -4610,7 +4612,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="103" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A103" s="5">
         <v>2015</v>
       </c>
@@ -4633,7 +4635,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A104" s="5">
         <v>2015</v>
       </c>
@@ -4657,7 +4659,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="105" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A105" s="5">
         <v>2015</v>
       </c>
@@ -4680,7 +4682,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A106" s="5">
         <v>2015</v>
       </c>
@@ -4703,7 +4705,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A107" s="5">
         <v>2015</v>
       </c>
@@ -4727,7 +4729,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="108" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A108" s="5">
         <v>2016</v>
       </c>
@@ -4753,7 +4755,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="109" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A109" s="5">
         <v>2016</v>
       </c>
@@ -4776,7 +4778,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:8" s="5" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:8" s="5" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A110" s="5">
         <v>2016</v>
       </c>
@@ -4802,7 +4804,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="111" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A111" s="5">
         <v>2016</v>
       </c>
@@ -4825,7 +4827,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="112" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A112" s="5">
         <v>2017</v>
       </c>
@@ -4851,7 +4853,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="113" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A113" s="5">
         <v>2017</v>
       </c>
@@ -4875,7 +4877,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="114" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A114" s="5">
         <v>2017</v>
       </c>
@@ -4898,7 +4900,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="115" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A115" s="5">
         <v>2017</v>
       </c>
@@ -4921,7 +4923,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="116" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A116" s="5">
         <v>2017</v>
       </c>
@@ -4947,7 +4949,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="117" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="117" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A117" s="5">
         <v>2017</v>
       </c>
@@ -4970,7 +4972,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="118" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="118" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A118" s="5">
         <v>2017</v>
       </c>
@@ -4993,7 +4995,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="119" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="119" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A119" s="5">
         <v>2017</v>
       </c>
@@ -5017,7 +5019,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="120" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A120" s="5">
         <v>2017</v>
       </c>
@@ -5043,7 +5045,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="121" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="121" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A121" s="5">
         <v>2017</v>
       </c>
@@ -5066,7 +5068,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="122" spans="1:8" s="5" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+    <row r="122" spans="1:8" s="5" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A122" s="5">
         <v>2017</v>
       </c>
@@ -5092,7 +5094,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="123" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="123" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A123" s="5">
         <v>2017</v>
       </c>
@@ -5118,7 +5120,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="124" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="124" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A124" s="5">
         <v>2017</v>
       </c>
@@ -5144,7 +5146,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="125" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="125" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A125" s="5">
         <v>2017</v>
       </c>
@@ -5170,7 +5172,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="126" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="126" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A126" s="5">
         <v>2017</v>
       </c>
@@ -5193,7 +5195,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="127" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="127" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A127" s="5">
         <v>2018</v>
       </c>
@@ -5216,7 +5218,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="128" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="128" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A128" s="5">
         <v>2018</v>
       </c>
@@ -5242,7 +5244,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="129" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="129" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A129" s="5">
         <v>2018</v>
       </c>
@@ -5265,7 +5267,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="130" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="130" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A130" s="5">
         <v>2018</v>
       </c>
@@ -5291,7 +5293,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="131" spans="1:8" s="5" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+    <row r="131" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A131" s="5">
         <v>2018</v>
       </c>
@@ -5317,7 +5319,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="132" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="132" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A132" s="5">
         <v>2018</v>
       </c>
@@ -5340,7 +5342,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="133" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="133" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A133" s="5">
         <v>2018</v>
       </c>
@@ -5366,7 +5368,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="134" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="134" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A134" s="5">
         <v>2018</v>
       </c>
@@ -5390,7 +5392,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="135" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="135" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A135" s="5">
         <v>2018</v>
       </c>
@@ -5413,7 +5415,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="136" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="136" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A136" s="5">
         <v>2018</v>
       </c>
@@ -5439,7 +5441,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="137" spans="1:8" s="5" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+    <row r="137" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A137" s="5">
         <v>2018</v>
       </c>
@@ -5465,7 +5467,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="138" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="138" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A138" s="5">
         <v>2018</v>
       </c>
@@ -5491,7 +5493,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="139" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="139" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A139" s="5">
         <v>2018</v>
       </c>
@@ -5517,7 +5519,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="140" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="140" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A140" s="5">
         <v>2018</v>
       </c>
@@ -5541,7 +5543,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="141" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="141" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A141" s="5">
         <v>2018</v>
       </c>
@@ -5564,7 +5566,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="142" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="142" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A142" s="5">
         <v>2018</v>
       </c>
@@ -5587,7 +5589,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="143" spans="1:8" s="5" customFormat="1" ht="84" x14ac:dyDescent="0.15">
+    <row r="143" spans="1:8" s="5" customFormat="1" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A143" s="5">
         <v>2018</v>
       </c>
@@ -5613,7 +5615,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="144" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="144" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A144" s="5">
         <v>2019</v>
       </c>
@@ -5639,7 +5641,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="145" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="145" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A145" s="5">
         <v>2019</v>
       </c>
@@ -5662,7 +5664,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="146" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="146" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A146" s="5">
         <v>2019</v>
       </c>
@@ -5686,7 +5688,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="147" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="147" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A147" s="5">
         <v>2019</v>
       </c>
@@ -5712,7 +5714,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="148" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="148" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A148" s="5">
         <v>2019</v>
       </c>
@@ -5720,7 +5722,7 @@
         <v>274</v>
       </c>
       <c r="C148" s="5" t="s">
-        <v>460</v>
+        <v>474</v>
       </c>
       <c r="D148" s="5" t="s">
         <v>55</v>
@@ -5738,7 +5740,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="149" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="149" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A149" s="5">
         <v>2019</v>
       </c>
@@ -5762,7 +5764,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="150" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="150" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A150" s="5">
         <v>2019</v>
       </c>
@@ -5785,7 +5787,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="151" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="151" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A151" s="5">
         <v>2019</v>
       </c>
@@ -5808,7 +5810,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="152" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="152" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A152" s="5">
         <v>2019</v>
       </c>
@@ -5832,7 +5834,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="153" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="153" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A153" s="5">
         <v>2019</v>
       </c>
@@ -5858,7 +5860,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="154" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="154" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A154" s="5">
         <v>2019</v>
       </c>
@@ -5881,7 +5883,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="155" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="155" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A155" s="5">
         <v>2020</v>
       </c>
@@ -5907,7 +5909,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="156" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="156" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A156" s="5">
         <v>2020</v>
       </c>
@@ -5933,7 +5935,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="157" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="157" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A157" s="5">
         <v>2020</v>
       </c>
@@ -5956,7 +5958,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="158" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="158" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A158" s="5">
         <v>2020</v>
       </c>
@@ -5980,7 +5982,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="159" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="159" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A159" s="5">
         <v>2020</v>
       </c>
@@ -6006,7 +6008,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="160" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="160" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A160" s="5">
         <v>2020</v>
       </c>
@@ -6029,7 +6031,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="161" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="161" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A161" s="5">
         <v>2020</v>
       </c>
@@ -6055,7 +6057,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="162" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="162" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A162" s="5">
         <v>2020</v>
       </c>
@@ -6078,7 +6080,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="163" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="163" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A163" s="5">
         <v>2020</v>
       </c>
@@ -6101,7 +6103,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="164" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="164" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A164" s="5">
         <v>2020</v>
       </c>
@@ -6127,7 +6129,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="165" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="165" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A165" s="5">
         <v>2020</v>
       </c>
@@ -6147,7 +6149,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="166" spans="1:8" s="5" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+    <row r="166" spans="1:8" s="5" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A166" s="5">
         <v>2020</v>
       </c>
@@ -6173,7 +6175,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="167" spans="1:8" s="5" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+    <row r="167" spans="1:8" s="5" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A167" s="5">
         <v>2020</v>
       </c>
@@ -6199,7 +6201,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="168" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="168" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A168" s="5">
         <v>2020</v>
       </c>
@@ -6222,7 +6224,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="169" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="169" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A169" s="5">
         <v>2020</v>
       </c>
@@ -6230,7 +6232,7 @@
         <v>312</v>
       </c>
       <c r="C169" s="5" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D169" s="5" t="s">
         <v>55</v>
@@ -6248,7 +6250,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="170" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="170" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A170" s="5">
         <v>2020</v>
       </c>
@@ -6274,7 +6276,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="171" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="171" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A171" s="5">
         <v>2020</v>
       </c>
@@ -6300,7 +6302,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="172" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="172" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A172" s="5">
         <v>2020</v>
       </c>
@@ -6326,7 +6328,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="173" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="173" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A173" s="5">
         <v>2020</v>
       </c>
@@ -6350,7 +6352,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="174" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="174" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A174" s="5">
         <v>2020</v>
       </c>
@@ -6376,7 +6378,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="175" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="175" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A175" s="5">
         <v>2020</v>
       </c>
@@ -6402,7 +6404,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="176" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="176" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A176" s="5">
         <v>2021</v>
       </c>
@@ -6428,7 +6430,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="177" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="177" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A177" s="5">
         <v>2021</v>
       </c>
@@ -6454,7 +6456,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="178" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="178" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A178" s="5">
         <v>2021</v>
       </c>
@@ -6480,7 +6482,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="179" spans="1:8" s="5" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+    <row r="179" spans="1:8" s="5" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A179" s="5">
         <v>2021</v>
       </c>
@@ -6506,7 +6508,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="180" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="180" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A180" s="5">
         <v>2021</v>
       </c>
@@ -6529,7 +6531,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="181" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="181" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A181" s="5">
         <v>2021</v>
       </c>
@@ -6555,7 +6557,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="182" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="182" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A182" s="5">
         <v>2021</v>
       </c>
@@ -6579,7 +6581,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="183" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="183" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A183" s="5">
         <v>2021</v>
       </c>
@@ -6602,7 +6604,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="184" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="184" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A184" s="5">
         <v>2021</v>
       </c>
@@ -6625,7 +6627,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="185" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="185" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A185" s="5">
         <v>2021</v>
       </c>
@@ -6651,7 +6653,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="186" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="186" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A186" s="5">
         <v>2021</v>
       </c>
@@ -6674,7 +6676,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="187" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="187" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A187" s="5">
         <v>2021</v>
       </c>
@@ -6700,7 +6702,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="188" spans="1:8" s="5" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+    <row r="188" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A188" s="5">
         <v>2021</v>
       </c>
@@ -6726,7 +6728,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="189" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="189" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A189" s="5">
         <v>2021</v>
       </c>
@@ -6749,7 +6751,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="190" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="190" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A190" s="5">
         <v>2021</v>
       </c>
@@ -6772,7 +6774,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="191" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="191" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A191" s="5">
         <v>2021</v>
       </c>
@@ -6798,7 +6800,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="192" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="192" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A192" s="5">
         <v>2021</v>
       </c>
@@ -6821,7 +6823,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="193" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="193" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A193" s="5">
         <v>2022</v>
       </c>
@@ -6847,7 +6849,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="194" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="194" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A194" s="5">
         <v>2022</v>
       </c>
@@ -6871,7 +6873,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="195" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="195" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A195" s="5">
         <v>2022</v>
       </c>
@@ -6897,7 +6899,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="196" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="196" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A196" s="5">
         <v>2022</v>
       </c>
@@ -6923,7 +6925,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="197" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="197" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A197" s="5">
         <v>2022</v>
       </c>
@@ -6947,7 +6949,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="198" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="198" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A198" s="5">
         <v>2022</v>
       </c>
@@ -6970,7 +6972,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="199" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="199" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A199" s="5">
         <v>2022</v>
       </c>
@@ -6993,7 +6995,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="200" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="200" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A200" s="5">
         <v>2022</v>
       </c>
@@ -7019,7 +7021,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="201" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="201" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A201" s="5">
         <v>2022</v>
       </c>
@@ -7045,7 +7047,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="202" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="202" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A202" s="5">
         <v>2022</v>
       </c>
@@ -7071,7 +7073,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="203" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="203" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A203" s="5">
         <v>2022</v>
       </c>
@@ -7095,7 +7097,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="204" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="204" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A204" s="5">
         <v>2022</v>
       </c>
@@ -7118,7 +7120,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="205" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="205" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A205" s="5">
         <v>2023</v>
       </c>
@@ -7144,7 +7146,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="206" spans="1:8" s="5" customFormat="1" ht="42" x14ac:dyDescent="0.15">
+    <row r="206" spans="1:8" s="5" customFormat="1" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A206" s="5">
         <v>2023</v>
       </c>
@@ -7170,7 +7172,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="207" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="207" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A207" s="5">
         <v>2023</v>
       </c>
@@ -7193,7 +7195,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="208" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="208" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A208" s="5">
         <v>2023</v>
       </c>
@@ -7216,7 +7218,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="209" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="209" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A209" s="5">
         <v>2023</v>
       </c>
@@ -7240,7 +7242,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="210" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="210" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A210" s="5">
         <v>2023</v>
       </c>
@@ -7263,7 +7265,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="211" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="211" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A211" s="5">
         <v>2023</v>
       </c>
@@ -7286,7 +7288,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="212" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="212" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A212" s="5">
         <v>2023</v>
       </c>
@@ -7310,7 +7312,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="213" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="213" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A213" s="5">
         <v>2023</v>
       </c>
@@ -7336,7 +7338,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="214" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="214" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A214" s="5">
         <v>2023</v>
       </c>
@@ -7362,7 +7364,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="215" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="215" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A215" s="5">
         <v>2023</v>
       </c>
@@ -7386,7 +7388,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="216" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="216" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A216" s="5">
         <v>2023</v>
       </c>
@@ -7409,7 +7411,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="217" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="217" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A217" s="5">
         <v>2023</v>
       </c>
@@ -7432,18 +7434,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="218" spans="1:8" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="218" spans="1:8" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A218" s="5">
         <v>2023</v>
       </c>
       <c r="B218" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D218" s="5" t="s">
         <v>143</v>
       </c>
       <c r="E218" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="F218" s="5" t="s">
         <v>7</v>
@@ -7472,44 +7474,44 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="153.1640625" customWidth="1"/>
+    <col min="1" max="1" width="153.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="59" x14ac:dyDescent="0.2">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="55.8" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="45" x14ac:dyDescent="0.2">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="42.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
         <v>473</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>474</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update oncology tx page
</commit_message>
<xml_diff>
--- a/src/main/webapp/content/files/oncologyTherapies/fda_approved_oncology_therapies.xlsx
+++ b/src/main/webapp/content/files/oncologyTherapies/fda_approved_oncology_therapies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luc2\Desktop\oncokb\oncokb-public\src\main\webapp\content\files\oncologyTherapies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3D0D0C4-67AA-4683-9CD6-34CD80FD7BC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D45EF53A-463B-45D4-BCE1-BA0BB0E9A6C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6852" yWindow="2484" windowWidth="21816" windowHeight="13884" xr2:uid="{D862B214-800F-AF40-9BAA-60FE1781D5C8}"/>
+    <workbookView xWindow="4716" yWindow="576" windowWidth="21480" windowHeight="15456" xr2:uid="{D862B214-800F-AF40-9BAA-60FE1781D5C8}"/>
   </bookViews>
   <sheets>
     <sheet name="FDA-Approved Oncology Therapies" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1445" uniqueCount="483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1457" uniqueCount="488">
   <si>
     <t>Year of drug’s first FDA- approval</t>
   </si>
@@ -1707,6 +1707,21 @@
       </rPr>
       <t>d</t>
     </r>
+  </si>
+  <si>
+    <t>Tarlatamab</t>
+  </si>
+  <si>
+    <t>Bispecific DLL3-directed CD3 T-cell engager</t>
+  </si>
+  <si>
+    <t>Imetelstat</t>
+  </si>
+  <si>
+    <t>Telomerase inhibitor</t>
+  </si>
+  <si>
+    <t>Telomerase template antagonist</t>
   </si>
 </sst>
 </file>
@@ -2133,10 +2148,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B89377A-76F6-CA40-8081-AAD80BFAB6B8}">
-  <dimension ref="A1:H221"/>
+  <dimension ref="A1:H223"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A207" zoomScale="149" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B225" sqref="B225"/>
+      <selection activeCell="B227" sqref="B227"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -7554,6 +7569,54 @@
       </c>
       <c r="H221" s="2" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="222" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A222" s="5">
+        <v>2024</v>
+      </c>
+      <c r="B222" s="5" t="s">
+        <v>483</v>
+      </c>
+      <c r="C222" s="5"/>
+      <c r="D222" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="E222" s="5" t="s">
+        <v>484</v>
+      </c>
+      <c r="F222" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G222" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H222" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="223" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A223" s="5">
+        <v>2024</v>
+      </c>
+      <c r="B223" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="C223" s="5"/>
+      <c r="D223" s="5" t="s">
+        <v>486</v>
+      </c>
+      <c r="E223" s="5" t="s">
+        <v>487</v>
+      </c>
+      <c r="F223" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G223" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H223" s="5" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update news for v4.18 (#1131)
</commit_message>
<xml_diff>
--- a/src/main/webapp/content/files/oncologyTherapies/fda_approved_oncology_therapies.xlsx
+++ b/src/main/webapp/content/files/oncologyTherapies/fda_approved_oncology_therapies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luc2\Desktop\oncokb\oncokb-public\src\main\webapp\content\files\oncologyTherapies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3D0D0C4-67AA-4683-9CD6-34CD80FD7BC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D45EF53A-463B-45D4-BCE1-BA0BB0E9A6C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6852" yWindow="2484" windowWidth="21816" windowHeight="13884" xr2:uid="{D862B214-800F-AF40-9BAA-60FE1781D5C8}"/>
+    <workbookView xWindow="4716" yWindow="576" windowWidth="21480" windowHeight="15456" xr2:uid="{D862B214-800F-AF40-9BAA-60FE1781D5C8}"/>
   </bookViews>
   <sheets>
     <sheet name="FDA-Approved Oncology Therapies" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1445" uniqueCount="483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1457" uniqueCount="488">
   <si>
     <t>Year of drug’s first FDA- approval</t>
   </si>
@@ -1707,6 +1707,21 @@
       </rPr>
       <t>d</t>
     </r>
+  </si>
+  <si>
+    <t>Tarlatamab</t>
+  </si>
+  <si>
+    <t>Bispecific DLL3-directed CD3 T-cell engager</t>
+  </si>
+  <si>
+    <t>Imetelstat</t>
+  </si>
+  <si>
+    <t>Telomerase inhibitor</t>
+  </si>
+  <si>
+    <t>Telomerase template antagonist</t>
   </si>
 </sst>
 </file>
@@ -2133,10 +2148,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B89377A-76F6-CA40-8081-AAD80BFAB6B8}">
-  <dimension ref="A1:H221"/>
+  <dimension ref="A1:H223"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A207" zoomScale="149" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B225" sqref="B225"/>
+      <selection activeCell="B227" sqref="B227"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -7554,6 +7569,54 @@
       </c>
       <c r="H221" s="2" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="222" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A222" s="5">
+        <v>2024</v>
+      </c>
+      <c r="B222" s="5" t="s">
+        <v>483</v>
+      </c>
+      <c r="C222" s="5"/>
+      <c r="D222" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="E222" s="5" t="s">
+        <v>484</v>
+      </c>
+      <c r="F222" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G222" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H222" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="223" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A223" s="5">
+        <v>2024</v>
+      </c>
+      <c r="B223" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="C223" s="5"/>
+      <c r="D223" s="5" t="s">
+        <v>486</v>
+      </c>
+      <c r="E223" s="5" t="s">
+        <v>487</v>
+      </c>
+      <c r="F223" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G223" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H223" s="5" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update onc tx page
</commit_message>
<xml_diff>
--- a/src/main/webapp/content/files/oncologyTherapies/fda_approved_oncology_therapies.xlsx
+++ b/src/main/webapp/content/files/oncologyTherapies/fda_approved_oncology_therapies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luc2\Desktop\oncokb\oncokb-public\src\main\webapp\content\files\oncologyTherapies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luc2/Documents/oncokb/oncokb-public/src/main/webapp/content/files/oncologyTherapies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D45EF53A-463B-45D4-BCE1-BA0BB0E9A6C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3598799-5264-8C48-B722-891F8EC70695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4716" yWindow="576" windowWidth="21480" windowHeight="15456" xr2:uid="{D862B214-800F-AF40-9BAA-60FE1781D5C8}"/>
+    <workbookView xWindow="10600" yWindow="1480" windowWidth="33820" windowHeight="23700" xr2:uid="{D862B214-800F-AF40-9BAA-60FE1781D5C8}"/>
   </bookViews>
   <sheets>
     <sheet name="FDA-Approved Oncology Therapies" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1457" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1471" uniqueCount="495">
   <si>
     <t>Year of drug’s first FDA- approval</t>
   </si>
@@ -1722,6 +1722,27 @@
   </si>
   <si>
     <t>Telomerase template antagonist</t>
+  </si>
+  <si>
+    <t>Afamitresgene autoleucel</t>
+  </si>
+  <si>
+    <t>HLA-A*02:01P, -A*02:02P, -A*02:03P, or -A*02:06P positive and MAGE-A4 antigen positive</t>
+  </si>
+  <si>
+    <t>T cell receptor (TCR) therapy</t>
+  </si>
+  <si>
+    <t>MAGE-A4-directed TCR therapy</t>
+  </si>
+  <si>
+    <t>Vorasidenib</t>
+  </si>
+  <si>
+    <t>IDH1 R132H/C/G/S/L, IDH2 R172K/M/W/S/G</t>
+  </si>
+  <si>
+    <t>IDH1/IDH2 inhibitor</t>
   </si>
 </sst>
 </file>
@@ -2148,22 +2169,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B89377A-76F6-CA40-8081-AAD80BFAB6B8}">
-  <dimension ref="A1:H223"/>
+  <dimension ref="A1:H225"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A207" zoomScale="149" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B227" sqref="B227"/>
+      <selection activeCell="E225" sqref="E225"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.5" customWidth="1"/>
-    <col min="2" max="2" width="22.19921875" customWidth="1"/>
-    <col min="3" max="3" width="26.19921875" customWidth="1"/>
-    <col min="4" max="4" width="25.796875" customWidth="1"/>
-    <col min="5" max="5" width="27.296875" customWidth="1"/>
+    <col min="2" max="2" width="22.1640625" customWidth="1"/>
+    <col min="3" max="3" width="26.1640625" customWidth="1"/>
+    <col min="4" max="4" width="25.83203125" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2189,7 +2210,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -2212,7 +2233,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -2235,7 +2256,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -2261,7 +2282,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -2284,7 +2305,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -2307,7 +2328,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
@@ -2333,7 +2354,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -2356,7 +2377,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -2382,7 +2403,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>3</v>
       </c>
@@ -2408,7 +2429,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="2" customFormat="1" ht="66" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" s="2" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>3</v>
       </c>
@@ -2434,7 +2455,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
         <v>3</v>
       </c>
@@ -2457,7 +2478,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
         <v>3</v>
       </c>
@@ -2480,7 +2501,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
         <v>3</v>
       </c>
@@ -2506,7 +2527,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
         <v>3</v>
       </c>
@@ -2529,7 +2550,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
         <v>3</v>
       </c>
@@ -2552,7 +2573,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A17" s="2">
         <v>2002</v>
       </c>
@@ -2578,7 +2599,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A18" s="2">
         <v>2002</v>
       </c>
@@ -2601,7 +2622,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A19" s="2">
         <v>2002</v>
       </c>
@@ -2624,7 +2645,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A20" s="2">
         <v>2003</v>
       </c>
@@ -2648,7 +2669,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A21" s="2">
         <v>2003</v>
       </c>
@@ -2671,7 +2692,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A22" s="2">
         <v>2003</v>
       </c>
@@ -2697,7 +2718,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A23" s="2">
         <v>2003</v>
       </c>
@@ -2723,7 +2744,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A24" s="2">
         <v>2004</v>
       </c>
@@ -2746,7 +2767,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A25" s="2">
         <v>2004</v>
       </c>
@@ -2769,7 +2790,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:8" s="2" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" s="2" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A26" s="2">
         <v>2004</v>
       </c>
@@ -2795,7 +2816,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A27" s="2">
         <v>2004</v>
       </c>
@@ -2818,7 +2839,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A28" s="2">
         <v>2004</v>
       </c>
@@ -2844,7 +2865,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A29" s="2">
         <v>2004</v>
       </c>
@@ -2868,7 +2889,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A30" s="2">
         <v>2005</v>
       </c>
@@ -2891,7 +2912,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A31" s="2">
         <v>2005</v>
       </c>
@@ -2914,7 +2935,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A32" s="2">
         <v>2006</v>
       </c>
@@ -2940,7 +2961,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A33" s="2">
         <v>2006</v>
       </c>
@@ -2963,7 +2984,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A34" s="2">
         <v>2006</v>
       </c>
@@ -2986,7 +3007,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:8" s="2" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" s="2" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A35" s="2">
         <v>2006</v>
       </c>
@@ -3012,7 +3033,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A36" s="2">
         <v>2006</v>
       </c>
@@ -3038,7 +3059,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A37" s="2">
         <v>2006</v>
       </c>
@@ -3061,7 +3082,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A38" s="2">
         <v>2007</v>
       </c>
@@ -3085,7 +3106,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A39" s="2">
         <v>2007</v>
       </c>
@@ -3111,7 +3132,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A40" s="2">
         <v>2007</v>
       </c>
@@ -3137,7 +3158,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A41" s="2">
         <v>2007</v>
       </c>
@@ -3161,7 +3182,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A42" s="2">
         <v>2008</v>
       </c>
@@ -3184,7 +3205,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A43" s="2">
         <v>2008</v>
       </c>
@@ -3207,7 +3228,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" s="2" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A44" s="2">
         <v>2009</v>
       </c>
@@ -3233,7 +3254,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A45" s="2">
         <v>2009</v>
       </c>
@@ -3256,7 +3277,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A46" s="2">
         <v>2009</v>
       </c>
@@ -3279,7 +3300,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A47" s="2">
         <v>2009</v>
       </c>
@@ -3303,7 +3324,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A48" s="2">
         <v>2009</v>
       </c>
@@ -3326,7 +3347,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A49" s="2">
         <v>2010</v>
       </c>
@@ -3349,7 +3370,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A50" s="2">
         <v>2010</v>
       </c>
@@ -3373,7 +3394,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A51" s="2">
         <v>2010</v>
       </c>
@@ -3396,7 +3417,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A52" s="2">
         <v>2011</v>
       </c>
@@ -3419,7 +3440,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A53" s="2">
         <v>2011</v>
       </c>
@@ -3443,7 +3464,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A54" s="2">
         <v>2011</v>
       </c>
@@ -3469,7 +3490,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A55" s="2">
         <v>2011</v>
       </c>
@@ -3495,7 +3516,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A56" s="2">
         <v>2011</v>
       </c>
@@ -3519,7 +3540,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A57" s="2">
         <v>2011</v>
       </c>
@@ -3542,7 +3563,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A58" s="2">
         <v>2011</v>
       </c>
@@ -3565,7 +3586,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A59" s="2">
         <v>2011</v>
       </c>
@@ -3589,7 +3610,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A60" s="2">
         <v>2011</v>
       </c>
@@ -3615,7 +3636,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A61" s="2">
         <v>2012</v>
       </c>
@@ -3638,7 +3659,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A62" s="2">
         <v>2012</v>
       </c>
@@ -3662,7 +3683,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A63" s="2">
         <v>2012</v>
       </c>
@@ -3688,7 +3709,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A64" s="2">
         <v>2012</v>
       </c>
@@ -3711,7 +3732,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A65" s="2">
         <v>2012</v>
       </c>
@@ -3735,7 +3756,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A66" s="2">
         <v>2012</v>
       </c>
@@ -3758,7 +3779,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A67" s="2">
         <v>2012</v>
       </c>
@@ -3781,7 +3802,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A68" s="2">
         <v>2012</v>
       </c>
@@ -3807,7 +3828,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A69" s="2">
         <v>2012</v>
       </c>
@@ -3833,7 +3854,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A70" s="2">
         <v>2012</v>
       </c>
@@ -3859,7 +3880,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A71" s="2">
         <v>2012</v>
       </c>
@@ -3883,7 +3904,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A72" s="2">
         <v>2013</v>
       </c>
@@ -3909,7 +3930,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A73" s="2">
         <v>2013</v>
       </c>
@@ -3935,7 +3956,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A74" s="2">
         <v>2013</v>
       </c>
@@ -3961,7 +3982,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A75" s="2">
         <v>2013</v>
       </c>
@@ -3987,7 +4008,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A76" s="2">
         <v>2013</v>
       </c>
@@ -4010,7 +4031,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="77" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A77" s="2">
         <v>2013</v>
       </c>
@@ -4034,7 +4055,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A78" s="2">
         <v>2013</v>
       </c>
@@ -4057,7 +4078,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="79" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A79" s="2">
         <v>2013</v>
       </c>
@@ -4083,7 +4104,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A80" s="2">
         <v>2014</v>
       </c>
@@ -4107,7 +4128,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="81" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A81" s="2">
         <v>2014</v>
       </c>
@@ -4133,7 +4154,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="82" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A82" s="2">
         <v>2014</v>
       </c>
@@ -4159,7 +4180,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A83" s="2">
         <v>2014</v>
       </c>
@@ -4185,7 +4206,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A84" s="2">
         <v>2014</v>
       </c>
@@ -4208,7 +4229,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A85" s="2">
         <v>2014</v>
       </c>
@@ -4231,7 +4252,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="86" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A86" s="2">
         <v>2014</v>
       </c>
@@ -4255,7 +4276,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="87" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A87" s="2">
         <v>2014</v>
       </c>
@@ -4281,7 +4302,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="88" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A88" s="2">
         <v>2014</v>
       </c>
@@ -4307,7 +4328,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="89" spans="1:8" s="2" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" s="2" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A89" s="2">
         <v>2014</v>
       </c>
@@ -4333,7 +4354,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="90" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A90" s="2">
         <v>2014</v>
       </c>
@@ -4356,7 +4377,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="91" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A91" s="2">
         <v>2014</v>
       </c>
@@ -4379,7 +4400,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A92" s="2">
         <v>2015</v>
       </c>
@@ -4405,7 +4426,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="93" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A93" s="2">
         <v>2015</v>
       </c>
@@ -4431,7 +4452,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="94" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A94" s="2">
         <v>2015</v>
       </c>
@@ -4454,7 +4475,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A95" s="2">
         <v>2015</v>
       </c>
@@ -4478,7 +4499,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A96" s="2">
         <v>2015</v>
       </c>
@@ -4501,7 +4522,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A97" s="2">
         <v>2015</v>
       </c>
@@ -4527,7 +4548,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="98" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A98" s="2">
         <v>2015</v>
       </c>
@@ -4551,7 +4572,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A99" s="2">
         <v>2015</v>
       </c>
@@ -4574,7 +4595,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A100" s="2">
         <v>2015</v>
       </c>
@@ -4597,7 +4618,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="1:8" s="2" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" s="2" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A101" s="2">
         <v>2015</v>
       </c>
@@ -4623,7 +4644,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="102" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A102" s="2">
         <v>2015</v>
       </c>
@@ -4649,7 +4670,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="103" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A103" s="2">
         <v>2015</v>
       </c>
@@ -4672,7 +4693,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A104" s="2">
         <v>2015</v>
       </c>
@@ -4696,7 +4717,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="105" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A105" s="2">
         <v>2015</v>
       </c>
@@ -4719,7 +4740,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A106" s="2">
         <v>2015</v>
       </c>
@@ -4742,7 +4763,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A107" s="2">
         <v>2015</v>
       </c>
@@ -4766,7 +4787,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="108" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A108" s="2">
         <v>2016</v>
       </c>
@@ -4792,7 +4813,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="109" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A109" s="2">
         <v>2016</v>
       </c>
@@ -4815,7 +4836,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:8" s="2" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" s="2" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A110" s="2">
         <v>2016</v>
       </c>
@@ -4841,7 +4862,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="111" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A111" s="2">
         <v>2016</v>
       </c>
@@ -4864,7 +4885,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="112" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A112" s="2">
         <v>2017</v>
       </c>
@@ -4890,7 +4911,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="113" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A113" s="2">
         <v>2017</v>
       </c>
@@ -4914,7 +4935,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="114" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A114" s="2">
         <v>2017</v>
       </c>
@@ -4937,7 +4958,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A115" s="2">
         <v>2017</v>
       </c>
@@ -4960,7 +4981,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="116" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A116" s="2">
         <v>2017</v>
       </c>
@@ -4986,7 +5007,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="117" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A117" s="2">
         <v>2017</v>
       </c>
@@ -5009,7 +5030,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="118" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A118" s="2">
         <v>2017</v>
       </c>
@@ -5032,7 +5053,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="119" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A119" s="2">
         <v>2017</v>
       </c>
@@ -5056,7 +5077,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A120" s="2">
         <v>2017</v>
       </c>
@@ -5082,7 +5103,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="121" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A121" s="2">
         <v>2017</v>
       </c>
@@ -5108,7 +5129,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="122" spans="1:8" s="2" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" s="2" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A122" s="2">
         <v>2017</v>
       </c>
@@ -5134,7 +5155,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="123" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A123" s="2">
         <v>2017</v>
       </c>
@@ -5160,7 +5181,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="124" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A124" s="2">
         <v>2017</v>
       </c>
@@ -5186,7 +5207,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="125" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A125" s="2">
         <v>2017</v>
       </c>
@@ -5212,7 +5233,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="126" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A126" s="2">
         <v>2017</v>
       </c>
@@ -5235,7 +5256,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="127" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A127" s="2">
         <v>2018</v>
       </c>
@@ -5258,7 +5279,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="128" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A128" s="2">
         <v>2018</v>
       </c>
@@ -5284,7 +5305,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="129" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A129" s="2">
         <v>2018</v>
       </c>
@@ -5307,7 +5328,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="130" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A130" s="2">
         <v>2018</v>
       </c>
@@ -5333,7 +5354,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="131" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" s="2" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A131" s="2">
         <v>2018</v>
       </c>
@@ -5359,7 +5380,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="132" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A132" s="2">
         <v>2018</v>
       </c>
@@ -5382,7 +5403,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="133" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A133" s="2">
         <v>2018</v>
       </c>
@@ -5408,7 +5429,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="134" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A134" s="2">
         <v>2018</v>
       </c>
@@ -5432,7 +5453,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="135" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A135" s="2">
         <v>2018</v>
       </c>
@@ -5455,7 +5476,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="136" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A136" s="2">
         <v>2018</v>
       </c>
@@ -5481,7 +5502,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="137" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" s="2" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A137" s="2">
         <v>2018</v>
       </c>
@@ -5507,7 +5528,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="138" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A138" s="2">
         <v>2018</v>
       </c>
@@ -5533,7 +5554,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="139" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A139" s="2">
         <v>2018</v>
       </c>
@@ -5559,7 +5580,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="140" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A140" s="2">
         <v>2018</v>
       </c>
@@ -5583,7 +5604,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="141" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A141" s="2">
         <v>2018</v>
       </c>
@@ -5606,7 +5627,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="142" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A142" s="2">
         <v>2018</v>
       </c>
@@ -5629,7 +5650,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="143" spans="1:8" s="2" customFormat="1" ht="79.2" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" s="2" customFormat="1" ht="98" x14ac:dyDescent="0.15">
       <c r="A143" s="2">
         <v>2018</v>
       </c>
@@ -5655,7 +5676,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="144" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A144" s="2">
         <v>2019</v>
       </c>
@@ -5681,7 +5702,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="145" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A145" s="2">
         <v>2019</v>
       </c>
@@ -5704,7 +5725,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="146" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A146" s="2">
         <v>2019</v>
       </c>
@@ -5728,7 +5749,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="147" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A147" s="2">
         <v>2019</v>
       </c>
@@ -5754,7 +5775,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="148" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A148" s="2">
         <v>2019</v>
       </c>
@@ -5780,7 +5801,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="149" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A149" s="2">
         <v>2019</v>
       </c>
@@ -5804,7 +5825,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="150" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A150" s="2">
         <v>2019</v>
       </c>
@@ -5827,7 +5848,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="151" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A151" s="2">
         <v>2019</v>
       </c>
@@ -5850,7 +5871,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="152" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A152" s="2">
         <v>2019</v>
       </c>
@@ -5874,7 +5895,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="153" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A153" s="2">
         <v>2019</v>
       </c>
@@ -5900,7 +5921,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="154" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A154" s="2">
         <v>2019</v>
       </c>
@@ -5923,7 +5944,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="155" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A155" s="2">
         <v>2020</v>
       </c>
@@ -5949,7 +5970,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="156" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A156" s="2">
         <v>2020</v>
       </c>
@@ -5975,7 +5996,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="157" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A157" s="2">
         <v>2020</v>
       </c>
@@ -5998,7 +6019,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="158" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A158" s="2">
         <v>2020</v>
       </c>
@@ -6022,7 +6043,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="159" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A159" s="2">
         <v>2020</v>
       </c>
@@ -6048,7 +6069,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="160" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A160" s="2">
         <v>2020</v>
       </c>
@@ -6071,7 +6092,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="161" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A161" s="2">
         <v>2020</v>
       </c>
@@ -6097,7 +6118,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="162" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A162" s="2">
         <v>2020</v>
       </c>
@@ -6120,7 +6141,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="163" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A163" s="2">
         <v>2020</v>
       </c>
@@ -6143,7 +6164,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="164" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A164" s="2">
         <v>2020</v>
       </c>
@@ -6169,7 +6190,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="165" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A165" s="2">
         <v>2020</v>
       </c>
@@ -6189,7 +6210,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="166" spans="1:8" s="2" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8" s="2" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A166" s="2">
         <v>2020</v>
       </c>
@@ -6215,7 +6236,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="167" spans="1:8" s="2" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" s="2" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A167" s="2">
         <v>2020</v>
       </c>
@@ -6241,7 +6262,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="168" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A168" s="2">
         <v>2020</v>
       </c>
@@ -6264,7 +6285,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="169" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A169" s="2">
         <v>2020</v>
       </c>
@@ -6290,7 +6311,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="170" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A170" s="2">
         <v>2020</v>
       </c>
@@ -6316,7 +6337,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="171" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A171" s="2">
         <v>2020</v>
       </c>
@@ -6342,7 +6363,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="172" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A172" s="2">
         <v>2020</v>
       </c>
@@ -6368,7 +6389,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="173" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A173" s="2">
         <v>2020</v>
       </c>
@@ -6392,7 +6413,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="174" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A174" s="2">
         <v>2020</v>
       </c>
@@ -6418,7 +6439,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="175" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A175" s="2">
         <v>2020</v>
       </c>
@@ -6444,7 +6465,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="176" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A176" s="2">
         <v>2021</v>
       </c>
@@ -6470,7 +6491,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="177" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A177" s="2">
         <v>2021</v>
       </c>
@@ -6496,7 +6517,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="178" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A178" s="2">
         <v>2021</v>
       </c>
@@ -6522,7 +6543,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="179" spans="1:8" s="2" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:8" s="2" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A179" s="2">
         <v>2021</v>
       </c>
@@ -6548,7 +6569,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="180" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A180" s="2">
         <v>2021</v>
       </c>
@@ -6571,7 +6592,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="181" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A181" s="2">
         <v>2021</v>
       </c>
@@ -6597,7 +6618,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="182" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A182" s="2">
         <v>2021</v>
       </c>
@@ -6621,7 +6642,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="183" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A183" s="2">
         <v>2021</v>
       </c>
@@ -6644,7 +6665,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="184" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A184" s="2">
         <v>2021</v>
       </c>
@@ -6667,7 +6688,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="185" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A185" s="2">
         <v>2021</v>
       </c>
@@ -6693,7 +6714,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="186" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A186" s="2">
         <v>2021</v>
       </c>
@@ -6716,7 +6737,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="187" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A187" s="2">
         <v>2021</v>
       </c>
@@ -6742,7 +6763,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="188" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8" s="2" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A188" s="2">
         <v>2021</v>
       </c>
@@ -6768,7 +6789,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="189" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A189" s="2">
         <v>2021</v>
       </c>
@@ -6791,7 +6812,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="190" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A190" s="2">
         <v>2021</v>
       </c>
@@ -6814,7 +6835,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="191" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A191" s="2">
         <v>2021</v>
       </c>
@@ -6840,7 +6861,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="192" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A192" s="2">
         <v>2021</v>
       </c>
@@ -6863,7 +6884,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="193" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A193" s="2">
         <v>2022</v>
       </c>
@@ -6889,7 +6910,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="194" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A194" s="2">
         <v>2022</v>
       </c>
@@ -6913,7 +6934,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="195" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A195" s="2">
         <v>2022</v>
       </c>
@@ -6939,7 +6960,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="196" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A196" s="2">
         <v>2022</v>
       </c>
@@ -6965,7 +6986,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="197" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A197" s="2">
         <v>2022</v>
       </c>
@@ -6989,7 +7010,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="198" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A198" s="2">
         <v>2022</v>
       </c>
@@ -7012,7 +7033,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="199" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A199" s="2">
         <v>2022</v>
       </c>
@@ -7035,7 +7056,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="200" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A200" s="2">
         <v>2022</v>
       </c>
@@ -7061,7 +7082,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="201" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A201" s="2">
         <v>2022</v>
       </c>
@@ -7087,7 +7108,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="202" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A202" s="2">
         <v>2022</v>
       </c>
@@ -7113,7 +7134,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="203" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A203" s="2">
         <v>2022</v>
       </c>
@@ -7137,7 +7158,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="204" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A204" s="2">
         <v>2022</v>
       </c>
@@ -7160,7 +7181,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="205" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A205" s="2">
         <v>2023</v>
       </c>
@@ -7186,7 +7207,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="206" spans="1:8" s="2" customFormat="1" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:8" s="2" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A206" s="2">
         <v>2023</v>
       </c>
@@ -7212,7 +7233,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="207" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A207" s="2">
         <v>2023</v>
       </c>
@@ -7235,7 +7256,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="208" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A208" s="2">
         <v>2023</v>
       </c>
@@ -7258,7 +7279,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="209" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A209" s="2">
         <v>2023</v>
       </c>
@@ -7282,7 +7303,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="210" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A210" s="2">
         <v>2023</v>
       </c>
@@ -7305,7 +7326,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="211" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A211" s="2">
         <v>2023</v>
       </c>
@@ -7328,7 +7349,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="212" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A212" s="2">
         <v>2023</v>
       </c>
@@ -7352,7 +7373,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="213" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A213" s="2">
         <v>2023</v>
       </c>
@@ -7378,7 +7399,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="214" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A214" s="2">
         <v>2023</v>
       </c>
@@ -7404,7 +7425,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="215" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A215" s="2">
         <v>2023</v>
       </c>
@@ -7428,7 +7449,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="216" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A216" s="2">
         <v>2023</v>
       </c>
@@ -7451,7 +7472,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="217" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A217" s="2">
         <v>2023</v>
       </c>
@@ -7474,7 +7495,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="218" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A218" s="2">
         <v>2023</v>
       </c>
@@ -7497,7 +7518,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A219" s="2">
         <v>2024</v>
       </c>
@@ -7521,7 +7542,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A220" s="5">
         <v>2024</v>
       </c>
@@ -7545,7 +7566,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A221" s="2">
         <v>2024</v>
       </c>
@@ -7571,7 +7592,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A222" s="5">
         <v>2024</v>
       </c>
@@ -7595,7 +7616,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A223" s="5">
         <v>2024</v>
       </c>
@@ -7617,6 +7638,58 @@
       </c>
       <c r="H223" s="5" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="224" spans="1:8" ht="43" x14ac:dyDescent="0.2">
+      <c r="A224" s="3">
+        <v>2024</v>
+      </c>
+      <c r="B224" s="3" t="s">
+        <v>488</v>
+      </c>
+      <c r="C224" s="3" t="s">
+        <v>489</v>
+      </c>
+      <c r="D224" s="3" t="s">
+        <v>490</v>
+      </c>
+      <c r="E224" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="F224" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G224" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H224" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="225" spans="1:8" ht="29" x14ac:dyDescent="0.2">
+      <c r="A225" s="3">
+        <v>2024</v>
+      </c>
+      <c r="B225" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="C225" s="3" t="s">
+        <v>493</v>
+      </c>
+      <c r="D225" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E225" s="3" t="s">
+        <v>494</v>
+      </c>
+      <c r="F225" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G225" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H225" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -7636,42 +7709,42 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="153.19921875" customWidth="1"/>
+    <col min="1" max="1" width="153.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="55.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" ht="59" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="42.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" ht="45" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>468</v>
       </c>

</xml_diff>

<commit_message>
Update news 4.20 (#1142)
</commit_message>
<xml_diff>
--- a/src/main/webapp/content/files/oncologyTherapies/fda_approved_oncology_therapies.xlsx
+++ b/src/main/webapp/content/files/oncologyTherapies/fda_approved_oncology_therapies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luc2\Desktop\oncokb\oncokb-public\src\main\webapp\content\files\oncologyTherapies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luc2/Documents/oncokb/oncokb-public/src/main/webapp/content/files/oncologyTherapies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D45EF53A-463B-45D4-BCE1-BA0BB0E9A6C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3598799-5264-8C48-B722-891F8EC70695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4716" yWindow="576" windowWidth="21480" windowHeight="15456" xr2:uid="{D862B214-800F-AF40-9BAA-60FE1781D5C8}"/>
+    <workbookView xWindow="10600" yWindow="1480" windowWidth="33820" windowHeight="23700" xr2:uid="{D862B214-800F-AF40-9BAA-60FE1781D5C8}"/>
   </bookViews>
   <sheets>
     <sheet name="FDA-Approved Oncology Therapies" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1457" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1471" uniqueCount="495">
   <si>
     <t>Year of drug’s first FDA- approval</t>
   </si>
@@ -1722,6 +1722,27 @@
   </si>
   <si>
     <t>Telomerase template antagonist</t>
+  </si>
+  <si>
+    <t>Afamitresgene autoleucel</t>
+  </si>
+  <si>
+    <t>HLA-A*02:01P, -A*02:02P, -A*02:03P, or -A*02:06P positive and MAGE-A4 antigen positive</t>
+  </si>
+  <si>
+    <t>T cell receptor (TCR) therapy</t>
+  </si>
+  <si>
+    <t>MAGE-A4-directed TCR therapy</t>
+  </si>
+  <si>
+    <t>Vorasidenib</t>
+  </si>
+  <si>
+    <t>IDH1 R132H/C/G/S/L, IDH2 R172K/M/W/S/G</t>
+  </si>
+  <si>
+    <t>IDH1/IDH2 inhibitor</t>
   </si>
 </sst>
 </file>
@@ -2148,22 +2169,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B89377A-76F6-CA40-8081-AAD80BFAB6B8}">
-  <dimension ref="A1:H223"/>
+  <dimension ref="A1:H225"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A207" zoomScale="149" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B227" sqref="B227"/>
+      <selection activeCell="E225" sqref="E225"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.5" customWidth="1"/>
-    <col min="2" max="2" width="22.19921875" customWidth="1"/>
-    <col min="3" max="3" width="26.19921875" customWidth="1"/>
-    <col min="4" max="4" width="25.796875" customWidth="1"/>
-    <col min="5" max="5" width="27.296875" customWidth="1"/>
+    <col min="2" max="2" width="22.1640625" customWidth="1"/>
+    <col min="3" max="3" width="26.1640625" customWidth="1"/>
+    <col min="4" max="4" width="25.83203125" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2189,7 +2210,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -2212,7 +2233,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -2235,7 +2256,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -2261,7 +2282,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -2284,7 +2305,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -2307,7 +2328,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
@@ -2333,7 +2354,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -2356,7 +2377,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -2382,7 +2403,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>3</v>
       </c>
@@ -2408,7 +2429,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="2" customFormat="1" ht="66" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" s="2" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>3</v>
       </c>
@@ -2434,7 +2455,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
         <v>3</v>
       </c>
@@ -2457,7 +2478,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
         <v>3</v>
       </c>
@@ -2480,7 +2501,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
         <v>3</v>
       </c>
@@ -2506,7 +2527,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
         <v>3</v>
       </c>
@@ -2529,7 +2550,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
         <v>3</v>
       </c>
@@ -2552,7 +2573,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A17" s="2">
         <v>2002</v>
       </c>
@@ -2578,7 +2599,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A18" s="2">
         <v>2002</v>
       </c>
@@ -2601,7 +2622,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A19" s="2">
         <v>2002</v>
       </c>
@@ -2624,7 +2645,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A20" s="2">
         <v>2003</v>
       </c>
@@ -2648,7 +2669,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A21" s="2">
         <v>2003</v>
       </c>
@@ -2671,7 +2692,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A22" s="2">
         <v>2003</v>
       </c>
@@ -2697,7 +2718,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A23" s="2">
         <v>2003</v>
       </c>
@@ -2723,7 +2744,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A24" s="2">
         <v>2004</v>
       </c>
@@ -2746,7 +2767,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A25" s="2">
         <v>2004</v>
       </c>
@@ -2769,7 +2790,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:8" s="2" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" s="2" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A26" s="2">
         <v>2004</v>
       </c>
@@ -2795,7 +2816,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A27" s="2">
         <v>2004</v>
       </c>
@@ -2818,7 +2839,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A28" s="2">
         <v>2004</v>
       </c>
@@ -2844,7 +2865,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A29" s="2">
         <v>2004</v>
       </c>
@@ -2868,7 +2889,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A30" s="2">
         <v>2005</v>
       </c>
@@ -2891,7 +2912,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A31" s="2">
         <v>2005</v>
       </c>
@@ -2914,7 +2935,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A32" s="2">
         <v>2006</v>
       </c>
@@ -2940,7 +2961,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A33" s="2">
         <v>2006</v>
       </c>
@@ -2963,7 +2984,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A34" s="2">
         <v>2006</v>
       </c>
@@ -2986,7 +3007,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:8" s="2" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" s="2" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A35" s="2">
         <v>2006</v>
       </c>
@@ -3012,7 +3033,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A36" s="2">
         <v>2006</v>
       </c>
@@ -3038,7 +3059,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A37" s="2">
         <v>2006</v>
       </c>
@@ -3061,7 +3082,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A38" s="2">
         <v>2007</v>
       </c>
@@ -3085,7 +3106,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A39" s="2">
         <v>2007</v>
       </c>
@@ -3111,7 +3132,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A40" s="2">
         <v>2007</v>
       </c>
@@ -3137,7 +3158,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A41" s="2">
         <v>2007</v>
       </c>
@@ -3161,7 +3182,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A42" s="2">
         <v>2008</v>
       </c>
@@ -3184,7 +3205,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A43" s="2">
         <v>2008</v>
       </c>
@@ -3207,7 +3228,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" s="2" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A44" s="2">
         <v>2009</v>
       </c>
@@ -3233,7 +3254,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A45" s="2">
         <v>2009</v>
       </c>
@@ -3256,7 +3277,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A46" s="2">
         <v>2009</v>
       </c>
@@ -3279,7 +3300,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A47" s="2">
         <v>2009</v>
       </c>
@@ -3303,7 +3324,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A48" s="2">
         <v>2009</v>
       </c>
@@ -3326,7 +3347,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A49" s="2">
         <v>2010</v>
       </c>
@@ -3349,7 +3370,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A50" s="2">
         <v>2010</v>
       </c>
@@ -3373,7 +3394,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A51" s="2">
         <v>2010</v>
       </c>
@@ -3396,7 +3417,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A52" s="2">
         <v>2011</v>
       </c>
@@ -3419,7 +3440,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A53" s="2">
         <v>2011</v>
       </c>
@@ -3443,7 +3464,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A54" s="2">
         <v>2011</v>
       </c>
@@ -3469,7 +3490,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A55" s="2">
         <v>2011</v>
       </c>
@@ -3495,7 +3516,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A56" s="2">
         <v>2011</v>
       </c>
@@ -3519,7 +3540,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A57" s="2">
         <v>2011</v>
       </c>
@@ -3542,7 +3563,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A58" s="2">
         <v>2011</v>
       </c>
@@ -3565,7 +3586,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A59" s="2">
         <v>2011</v>
       </c>
@@ -3589,7 +3610,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A60" s="2">
         <v>2011</v>
       </c>
@@ -3615,7 +3636,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A61" s="2">
         <v>2012</v>
       </c>
@@ -3638,7 +3659,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A62" s="2">
         <v>2012</v>
       </c>
@@ -3662,7 +3683,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A63" s="2">
         <v>2012</v>
       </c>
@@ -3688,7 +3709,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A64" s="2">
         <v>2012</v>
       </c>
@@ -3711,7 +3732,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A65" s="2">
         <v>2012</v>
       </c>
@@ -3735,7 +3756,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A66" s="2">
         <v>2012</v>
       </c>
@@ -3758,7 +3779,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A67" s="2">
         <v>2012</v>
       </c>
@@ -3781,7 +3802,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A68" s="2">
         <v>2012</v>
       </c>
@@ -3807,7 +3828,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A69" s="2">
         <v>2012</v>
       </c>
@@ -3833,7 +3854,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A70" s="2">
         <v>2012</v>
       </c>
@@ -3859,7 +3880,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A71" s="2">
         <v>2012</v>
       </c>
@@ -3883,7 +3904,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A72" s="2">
         <v>2013</v>
       </c>
@@ -3909,7 +3930,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A73" s="2">
         <v>2013</v>
       </c>
@@ -3935,7 +3956,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A74" s="2">
         <v>2013</v>
       </c>
@@ -3961,7 +3982,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A75" s="2">
         <v>2013</v>
       </c>
@@ -3987,7 +4008,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A76" s="2">
         <v>2013</v>
       </c>
@@ -4010,7 +4031,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="77" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A77" s="2">
         <v>2013</v>
       </c>
@@ -4034,7 +4055,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A78" s="2">
         <v>2013</v>
       </c>
@@ -4057,7 +4078,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="79" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A79" s="2">
         <v>2013</v>
       </c>
@@ -4083,7 +4104,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A80" s="2">
         <v>2014</v>
       </c>
@@ -4107,7 +4128,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="81" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A81" s="2">
         <v>2014</v>
       </c>
@@ -4133,7 +4154,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="82" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A82" s="2">
         <v>2014</v>
       </c>
@@ -4159,7 +4180,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A83" s="2">
         <v>2014</v>
       </c>
@@ -4185,7 +4206,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A84" s="2">
         <v>2014</v>
       </c>
@@ -4208,7 +4229,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A85" s="2">
         <v>2014</v>
       </c>
@@ -4231,7 +4252,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="86" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A86" s="2">
         <v>2014</v>
       </c>
@@ -4255,7 +4276,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="87" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A87" s="2">
         <v>2014</v>
       </c>
@@ -4281,7 +4302,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="88" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A88" s="2">
         <v>2014</v>
       </c>
@@ -4307,7 +4328,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="89" spans="1:8" s="2" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" s="2" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A89" s="2">
         <v>2014</v>
       </c>
@@ -4333,7 +4354,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="90" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A90" s="2">
         <v>2014</v>
       </c>
@@ -4356,7 +4377,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="91" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A91" s="2">
         <v>2014</v>
       </c>
@@ -4379,7 +4400,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A92" s="2">
         <v>2015</v>
       </c>
@@ -4405,7 +4426,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="93" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A93" s="2">
         <v>2015</v>
       </c>
@@ -4431,7 +4452,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="94" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A94" s="2">
         <v>2015</v>
       </c>
@@ -4454,7 +4475,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A95" s="2">
         <v>2015</v>
       </c>
@@ -4478,7 +4499,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A96" s="2">
         <v>2015</v>
       </c>
@@ -4501,7 +4522,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A97" s="2">
         <v>2015</v>
       </c>
@@ -4527,7 +4548,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="98" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A98" s="2">
         <v>2015</v>
       </c>
@@ -4551,7 +4572,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A99" s="2">
         <v>2015</v>
       </c>
@@ -4574,7 +4595,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A100" s="2">
         <v>2015</v>
       </c>
@@ -4597,7 +4618,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="1:8" s="2" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" s="2" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A101" s="2">
         <v>2015</v>
       </c>
@@ -4623,7 +4644,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="102" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A102" s="2">
         <v>2015</v>
       </c>
@@ -4649,7 +4670,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="103" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A103" s="2">
         <v>2015</v>
       </c>
@@ -4672,7 +4693,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A104" s="2">
         <v>2015</v>
       </c>
@@ -4696,7 +4717,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="105" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A105" s="2">
         <v>2015</v>
       </c>
@@ -4719,7 +4740,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A106" s="2">
         <v>2015</v>
       </c>
@@ -4742,7 +4763,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A107" s="2">
         <v>2015</v>
       </c>
@@ -4766,7 +4787,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="108" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A108" s="2">
         <v>2016</v>
       </c>
@@ -4792,7 +4813,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="109" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A109" s="2">
         <v>2016</v>
       </c>
@@ -4815,7 +4836,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:8" s="2" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" s="2" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A110" s="2">
         <v>2016</v>
       </c>
@@ -4841,7 +4862,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="111" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A111" s="2">
         <v>2016</v>
       </c>
@@ -4864,7 +4885,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="112" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A112" s="2">
         <v>2017</v>
       </c>
@@ -4890,7 +4911,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="113" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A113" s="2">
         <v>2017</v>
       </c>
@@ -4914,7 +4935,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="114" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A114" s="2">
         <v>2017</v>
       </c>
@@ -4937,7 +4958,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A115" s="2">
         <v>2017</v>
       </c>
@@ -4960,7 +4981,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="116" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A116" s="2">
         <v>2017</v>
       </c>
@@ -4986,7 +5007,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="117" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A117" s="2">
         <v>2017</v>
       </c>
@@ -5009,7 +5030,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="118" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A118" s="2">
         <v>2017</v>
       </c>
@@ -5032,7 +5053,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="119" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A119" s="2">
         <v>2017</v>
       </c>
@@ -5056,7 +5077,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A120" s="2">
         <v>2017</v>
       </c>
@@ -5082,7 +5103,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="121" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A121" s="2">
         <v>2017</v>
       </c>
@@ -5108,7 +5129,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="122" spans="1:8" s="2" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" s="2" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A122" s="2">
         <v>2017</v>
       </c>
@@ -5134,7 +5155,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="123" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A123" s="2">
         <v>2017</v>
       </c>
@@ -5160,7 +5181,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="124" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A124" s="2">
         <v>2017</v>
       </c>
@@ -5186,7 +5207,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="125" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A125" s="2">
         <v>2017</v>
       </c>
@@ -5212,7 +5233,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="126" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A126" s="2">
         <v>2017</v>
       </c>
@@ -5235,7 +5256,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="127" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A127" s="2">
         <v>2018</v>
       </c>
@@ -5258,7 +5279,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="128" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A128" s="2">
         <v>2018</v>
       </c>
@@ -5284,7 +5305,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="129" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A129" s="2">
         <v>2018</v>
       </c>
@@ -5307,7 +5328,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="130" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A130" s="2">
         <v>2018</v>
       </c>
@@ -5333,7 +5354,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="131" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" s="2" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A131" s="2">
         <v>2018</v>
       </c>
@@ -5359,7 +5380,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="132" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A132" s="2">
         <v>2018</v>
       </c>
@@ -5382,7 +5403,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="133" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A133" s="2">
         <v>2018</v>
       </c>
@@ -5408,7 +5429,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="134" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A134" s="2">
         <v>2018</v>
       </c>
@@ -5432,7 +5453,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="135" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A135" s="2">
         <v>2018</v>
       </c>
@@ -5455,7 +5476,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="136" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A136" s="2">
         <v>2018</v>
       </c>
@@ -5481,7 +5502,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="137" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" s="2" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A137" s="2">
         <v>2018</v>
       </c>
@@ -5507,7 +5528,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="138" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A138" s="2">
         <v>2018</v>
       </c>
@@ -5533,7 +5554,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="139" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A139" s="2">
         <v>2018</v>
       </c>
@@ -5559,7 +5580,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="140" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A140" s="2">
         <v>2018</v>
       </c>
@@ -5583,7 +5604,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="141" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A141" s="2">
         <v>2018</v>
       </c>
@@ -5606,7 +5627,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="142" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A142" s="2">
         <v>2018</v>
       </c>
@@ -5629,7 +5650,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="143" spans="1:8" s="2" customFormat="1" ht="79.2" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" s="2" customFormat="1" ht="98" x14ac:dyDescent="0.15">
       <c r="A143" s="2">
         <v>2018</v>
       </c>
@@ -5655,7 +5676,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="144" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A144" s="2">
         <v>2019</v>
       </c>
@@ -5681,7 +5702,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="145" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A145" s="2">
         <v>2019</v>
       </c>
@@ -5704,7 +5725,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="146" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A146" s="2">
         <v>2019</v>
       </c>
@@ -5728,7 +5749,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="147" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A147" s="2">
         <v>2019</v>
       </c>
@@ -5754,7 +5775,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="148" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A148" s="2">
         <v>2019</v>
       </c>
@@ -5780,7 +5801,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="149" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A149" s="2">
         <v>2019</v>
       </c>
@@ -5804,7 +5825,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="150" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A150" s="2">
         <v>2019</v>
       </c>
@@ -5827,7 +5848,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="151" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A151" s="2">
         <v>2019</v>
       </c>
@@ -5850,7 +5871,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="152" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A152" s="2">
         <v>2019</v>
       </c>
@@ -5874,7 +5895,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="153" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A153" s="2">
         <v>2019</v>
       </c>
@@ -5900,7 +5921,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="154" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A154" s="2">
         <v>2019</v>
       </c>
@@ -5923,7 +5944,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="155" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A155" s="2">
         <v>2020</v>
       </c>
@@ -5949,7 +5970,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="156" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A156" s="2">
         <v>2020</v>
       </c>
@@ -5975,7 +5996,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="157" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A157" s="2">
         <v>2020</v>
       </c>
@@ -5998,7 +6019,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="158" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A158" s="2">
         <v>2020</v>
       </c>
@@ -6022,7 +6043,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="159" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A159" s="2">
         <v>2020</v>
       </c>
@@ -6048,7 +6069,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="160" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A160" s="2">
         <v>2020</v>
       </c>
@@ -6071,7 +6092,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="161" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A161" s="2">
         <v>2020</v>
       </c>
@@ -6097,7 +6118,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="162" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A162" s="2">
         <v>2020</v>
       </c>
@@ -6120,7 +6141,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="163" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A163" s="2">
         <v>2020</v>
       </c>
@@ -6143,7 +6164,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="164" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A164" s="2">
         <v>2020</v>
       </c>
@@ -6169,7 +6190,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="165" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A165" s="2">
         <v>2020</v>
       </c>
@@ -6189,7 +6210,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="166" spans="1:8" s="2" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8" s="2" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A166" s="2">
         <v>2020</v>
       </c>
@@ -6215,7 +6236,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="167" spans="1:8" s="2" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" s="2" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A167" s="2">
         <v>2020</v>
       </c>
@@ -6241,7 +6262,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="168" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A168" s="2">
         <v>2020</v>
       </c>
@@ -6264,7 +6285,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="169" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A169" s="2">
         <v>2020</v>
       </c>
@@ -6290,7 +6311,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="170" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A170" s="2">
         <v>2020</v>
       </c>
@@ -6316,7 +6337,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="171" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A171" s="2">
         <v>2020</v>
       </c>
@@ -6342,7 +6363,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="172" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A172" s="2">
         <v>2020</v>
       </c>
@@ -6368,7 +6389,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="173" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A173" s="2">
         <v>2020</v>
       </c>
@@ -6392,7 +6413,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="174" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A174" s="2">
         <v>2020</v>
       </c>
@@ -6418,7 +6439,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="175" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A175" s="2">
         <v>2020</v>
       </c>
@@ -6444,7 +6465,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="176" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A176" s="2">
         <v>2021</v>
       </c>
@@ -6470,7 +6491,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="177" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A177" s="2">
         <v>2021</v>
       </c>
@@ -6496,7 +6517,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="178" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A178" s="2">
         <v>2021</v>
       </c>
@@ -6522,7 +6543,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="179" spans="1:8" s="2" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:8" s="2" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A179" s="2">
         <v>2021</v>
       </c>
@@ -6548,7 +6569,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="180" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A180" s="2">
         <v>2021</v>
       </c>
@@ -6571,7 +6592,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="181" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A181" s="2">
         <v>2021</v>
       </c>
@@ -6597,7 +6618,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="182" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A182" s="2">
         <v>2021</v>
       </c>
@@ -6621,7 +6642,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="183" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A183" s="2">
         <v>2021</v>
       </c>
@@ -6644,7 +6665,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="184" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A184" s="2">
         <v>2021</v>
       </c>
@@ -6667,7 +6688,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="185" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A185" s="2">
         <v>2021</v>
       </c>
@@ -6693,7 +6714,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="186" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A186" s="2">
         <v>2021</v>
       </c>
@@ -6716,7 +6737,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="187" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A187" s="2">
         <v>2021</v>
       </c>
@@ -6742,7 +6763,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="188" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8" s="2" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A188" s="2">
         <v>2021</v>
       </c>
@@ -6768,7 +6789,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="189" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A189" s="2">
         <v>2021</v>
       </c>
@@ -6791,7 +6812,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="190" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A190" s="2">
         <v>2021</v>
       </c>
@@ -6814,7 +6835,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="191" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A191" s="2">
         <v>2021</v>
       </c>
@@ -6840,7 +6861,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="192" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A192" s="2">
         <v>2021</v>
       </c>
@@ -6863,7 +6884,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="193" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A193" s="2">
         <v>2022</v>
       </c>
@@ -6889,7 +6910,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="194" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A194" s="2">
         <v>2022</v>
       </c>
@@ -6913,7 +6934,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="195" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A195" s="2">
         <v>2022</v>
       </c>
@@ -6939,7 +6960,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="196" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A196" s="2">
         <v>2022</v>
       </c>
@@ -6965,7 +6986,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="197" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A197" s="2">
         <v>2022</v>
       </c>
@@ -6989,7 +7010,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="198" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A198" s="2">
         <v>2022</v>
       </c>
@@ -7012,7 +7033,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="199" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A199" s="2">
         <v>2022</v>
       </c>
@@ -7035,7 +7056,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="200" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A200" s="2">
         <v>2022</v>
       </c>
@@ -7061,7 +7082,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="201" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A201" s="2">
         <v>2022</v>
       </c>
@@ -7087,7 +7108,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="202" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A202" s="2">
         <v>2022</v>
       </c>
@@ -7113,7 +7134,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="203" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A203" s="2">
         <v>2022</v>
       </c>
@@ -7137,7 +7158,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="204" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A204" s="2">
         <v>2022</v>
       </c>
@@ -7160,7 +7181,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="205" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A205" s="2">
         <v>2023</v>
       </c>
@@ -7186,7 +7207,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="206" spans="1:8" s="2" customFormat="1" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:8" s="2" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A206" s="2">
         <v>2023</v>
       </c>
@@ -7212,7 +7233,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="207" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A207" s="2">
         <v>2023</v>
       </c>
@@ -7235,7 +7256,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="208" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A208" s="2">
         <v>2023</v>
       </c>
@@ -7258,7 +7279,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="209" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A209" s="2">
         <v>2023</v>
       </c>
@@ -7282,7 +7303,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="210" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A210" s="2">
         <v>2023</v>
       </c>
@@ -7305,7 +7326,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="211" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A211" s="2">
         <v>2023</v>
       </c>
@@ -7328,7 +7349,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="212" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A212" s="2">
         <v>2023</v>
       </c>
@@ -7352,7 +7373,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="213" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A213" s="2">
         <v>2023</v>
       </c>
@@ -7378,7 +7399,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="214" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A214" s="2">
         <v>2023</v>
       </c>
@@ -7404,7 +7425,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="215" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:8" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A215" s="2">
         <v>2023</v>
       </c>
@@ -7428,7 +7449,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="216" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A216" s="2">
         <v>2023</v>
       </c>
@@ -7451,7 +7472,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="217" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A217" s="2">
         <v>2023</v>
       </c>
@@ -7474,7 +7495,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="218" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A218" s="2">
         <v>2023</v>
       </c>
@@ -7497,7 +7518,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A219" s="2">
         <v>2024</v>
       </c>
@@ -7521,7 +7542,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A220" s="5">
         <v>2024</v>
       </c>
@@ -7545,7 +7566,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A221" s="2">
         <v>2024</v>
       </c>
@@ -7571,7 +7592,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A222" s="5">
         <v>2024</v>
       </c>
@@ -7595,7 +7616,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A223" s="5">
         <v>2024</v>
       </c>
@@ -7617,6 +7638,58 @@
       </c>
       <c r="H223" s="5" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="224" spans="1:8" ht="43" x14ac:dyDescent="0.2">
+      <c r="A224" s="3">
+        <v>2024</v>
+      </c>
+      <c r="B224" s="3" t="s">
+        <v>488</v>
+      </c>
+      <c r="C224" s="3" t="s">
+        <v>489</v>
+      </c>
+      <c r="D224" s="3" t="s">
+        <v>490</v>
+      </c>
+      <c r="E224" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="F224" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G224" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H224" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="225" spans="1:8" ht="29" x14ac:dyDescent="0.2">
+      <c r="A225" s="3">
+        <v>2024</v>
+      </c>
+      <c r="B225" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="C225" s="3" t="s">
+        <v>493</v>
+      </c>
+      <c r="D225" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E225" s="3" t="s">
+        <v>494</v>
+      </c>
+      <c r="F225" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G225" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H225" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -7636,42 +7709,42 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="153.19921875" customWidth="1"/>
+    <col min="1" max="1" width="153.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="55.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" ht="59" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="42.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" ht="45" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>468</v>
       </c>

</xml_diff>

<commit_message>
Add news for 5.1
</commit_message>
<xml_diff>
--- a/src/main/webapp/content/files/oncologyTherapies/fda_approved_oncology_therapies.xlsx
+++ b/src/main/webapp/content/files/oncologyTherapies/fda_approved_oncology_therapies.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mskcc-my.sharepoint.com/personal/phillis2_mskcc_org/Documents/Precision Oncology Drug Page for Website/FDA-Approved_Oncology_therapies_bi_monthly updates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cavendk1/Documents/New onc therapies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{8C0F3825-168A-3C4C-913E-753BB014F271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33F0D526-34CA-1149-A4CE-440D95A17625}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59E48DA2-5F66-174E-9D87-A0BE250055A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="49820" yWindow="2800" windowWidth="29560" windowHeight="16900" xr2:uid="{D862B214-800F-AF40-9BAA-60FE1781D5C8}"/>
+    <workbookView xWindow="3480" yWindow="-21100" windowWidth="30240" windowHeight="17460" xr2:uid="{D862B214-800F-AF40-9BAA-60FE1781D5C8}"/>
   </bookViews>
   <sheets>
     <sheet name="FDA-Approved Oncology Therapies" sheetId="1" r:id="rId1"/>
     <sheet name="Footnotes" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'FDA-Approved Oncology Therapies'!$A$1:$H$243</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'FDA-Approved Oncology Therapies'!$A$1:$I$247</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1595" uniqueCount="532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1622" uniqueCount="543">
   <si>
     <t>Year of drug’s first FDA- approval</t>
   </si>
@@ -728,9 +728,6 @@
   </si>
   <si>
     <t>Neratinib</t>
-  </si>
-  <si>
-    <t>EGFR//HER2 (ERBB2)/HER4 (ERBB4) inhibitor</t>
   </si>
   <si>
     <t>Niraparib</t>
@@ -1708,9 +1705,6 @@
     <t>dMMR</t>
   </si>
   <si>
-    <t>Bispecific HER2/HER3-directed T-cell engager</t>
-  </si>
-  <si>
     <t>Menin inhibitor</t>
   </si>
   <si>
@@ -1845,6 +1839,46 @@
   </si>
   <si>
     <t>Telisotuzumab</t>
+  </si>
+  <si>
+    <t>*HR+/HER2-
+*EGFR Oncogenic Mutations</t>
+  </si>
+  <si>
+    <t>Linvoseltamab</t>
+  </si>
+  <si>
+    <t>Bispecific antibody</t>
+  </si>
+  <si>
+    <t>Bispecific HER2/HER3 antibody</t>
+  </si>
+  <si>
+    <t>Sunvozertinib</t>
+  </si>
+  <si>
+    <t>Dordaviprone</t>
+  </si>
+  <si>
+    <t>Protease activator</t>
+  </si>
+  <si>
+    <t>H3 K27M (K28M): H3-3A (H3F3A), H3C2 (HIST1H3B), H3C3 (HIST1H3C)</t>
+  </si>
+  <si>
+    <t>DRD2 and ClpP agonist</t>
+  </si>
+  <si>
+    <t>Zongertinib</t>
+  </si>
+  <si>
+    <t>ERBB2 TKD activating mutations</t>
+  </si>
+  <si>
+    <t>HER2 (ERBB2) inhibitor</t>
+  </si>
+  <si>
+    <t>EGFR/HER2 (ERBB2)/HER4 (ERBB4) inhibitor</t>
   </si>
 </sst>
 </file>
@@ -1977,9 +2011,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1990,6 +2021,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2010,9 +2044,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2050,7 +2084,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2156,7 +2190,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2298,7 +2332,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2306,38 +2340,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B89377A-76F6-CA40-8081-AAD80BFAB6B8}">
-  <dimension ref="A1:I244"/>
+  <dimension ref="A1:I247"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A235" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B173" sqref="B173"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A230" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C245" sqref="C245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.1640625" customWidth="1"/>
-    <col min="2" max="2" width="26.1640625" style="12" customWidth="1"/>
-    <col min="3" max="3" width="27.83203125" style="12" customWidth="1"/>
-    <col min="4" max="4" width="29.5" style="12" customWidth="1"/>
-    <col min="5" max="5" width="77" style="12" customWidth="1"/>
+    <col min="2" max="2" width="26.1640625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" style="11" customWidth="1"/>
+    <col min="4" max="4" width="29.5" style="11" customWidth="1"/>
+    <col min="5" max="5" width="77" style="11" customWidth="1"/>
     <col min="10" max="16384" width="11.1640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="13" customFormat="1" ht="47" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="12" customFormat="1" ht="47" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>504</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>505</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>506</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="E1" s="8" t="s">
         <v>507</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>508</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>509</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>1</v>
@@ -2346,9 +2380,9 @@
         <v>2</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>477</v>
-      </c>
-      <c r="I1" s="12"/>
+        <v>476</v>
+      </c>
+      <c r="I1" s="11"/>
     </row>
     <row r="2" spans="1:9" s="5" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
@@ -2408,7 +2442,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>13</v>
@@ -2485,7 +2519,7 @@
         <v>19</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>20</v>
@@ -2537,7 +2571,7 @@
         <v>24</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>25</v>
@@ -2564,7 +2598,7 @@
         <v>27</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>20</v>
@@ -2588,16 +2622,16 @@
         <v>2018</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>54</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>6</v>
@@ -2668,7 +2702,7 @@
         <v>37</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>38</v>
@@ -2699,7 +2733,7 @@
         <v>25</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>6</v>
@@ -2745,7 +2779,7 @@
         <v>43</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>25</v>
@@ -2872,7 +2906,7 @@
         <v>53</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>54</v>
@@ -2899,7 +2933,7 @@
         <v>56</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>20</v>
@@ -2976,7 +3010,7 @@
         <v>60</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>38</v>
@@ -3028,7 +3062,7 @@
         <v>63</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>54</v>
@@ -3105,7 +3139,7 @@
         <v>29</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>30</v>
@@ -3129,14 +3163,14 @@
         <v>2019</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F32" s="7" t="s">
         <v>6</v>
@@ -3207,7 +3241,7 @@
         <v>73</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>38</v>
@@ -3231,16 +3265,16 @@
         <v>2019</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>54</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F36" s="7" t="s">
         <v>6</v>
@@ -3311,7 +3345,7 @@
         <v>81</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>54</v>
@@ -3338,7 +3372,7 @@
         <v>227</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>30</v>
@@ -3432,7 +3466,7 @@
       </c>
       <c r="I43" s="7"/>
     </row>
-    <row r="44" spans="1:9" s="5" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:9" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A44" s="7">
         <v>2009</v>
       </c>
@@ -3440,7 +3474,7 @@
         <v>90</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>86</v>
@@ -3489,14 +3523,14 @@
         <v>2019</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F46" s="7" t="s">
         <v>6</v>
@@ -3689,10 +3723,10 @@
         <v>2011</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>20</v>
@@ -3716,16 +3750,16 @@
         <v>2020</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>54</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F55" s="7" t="s">
         <v>6</v>
@@ -3818,16 +3852,16 @@
         <v>2019</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>54</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F59" s="7" t="s">
         <v>6</v>
@@ -3848,7 +3882,7 @@
         <v>118</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>54</v>
@@ -3922,14 +3956,14 @@
         <v>2021</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F63" s="7" t="s">
         <v>6</v>
@@ -3947,16 +3981,16 @@
         <v>2023</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>54</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="F64" s="7" t="s">
         <v>6</v>
@@ -4052,7 +4086,7 @@
         <v>133</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>134</v>
@@ -4071,7 +4105,7 @@
       </c>
       <c r="I68" s="7"/>
     </row>
-    <row r="69" spans="1:9" s="5" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:9" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A69" s="7">
         <v>2006</v>
       </c>
@@ -4079,7 +4113,7 @@
         <v>69</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>30</v>
@@ -4156,7 +4190,7 @@
         <v>143</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>144</v>
@@ -4183,7 +4217,7 @@
         <v>146</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>54</v>
@@ -4210,7 +4244,7 @@
         <v>147</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>54</v>
@@ -4237,7 +4271,7 @@
         <v>148</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>54</v>
@@ -4339,7 +4373,7 @@
         <v>156</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>54</v>
@@ -4391,7 +4425,7 @@
         <v>159</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>160</v>
@@ -4418,7 +4452,7 @@
         <v>162</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>54</v>
@@ -4445,7 +4479,7 @@
         <v>164</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>165</v>
@@ -4547,7 +4581,7 @@
         <v>173</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>109</v>
@@ -4574,7 +4608,7 @@
         <v>175</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>141</v>
@@ -4601,7 +4635,7 @@
         <v>177</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>109</v>
@@ -4678,7 +4712,7 @@
         <v>182</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>54</v>
@@ -4702,10 +4736,10 @@
         <v>2015</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>165</v>
@@ -4736,7 +4770,7 @@
         <v>20</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F94" s="7" t="s">
         <v>6</v>
@@ -4807,7 +4841,7 @@
         <v>188</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D97" s="2" t="s">
         <v>109</v>
@@ -4856,14 +4890,14 @@
         <v>2021</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C99" s="2"/>
       <c r="D99" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F99" s="7" t="s">
         <v>6</v>
@@ -4909,7 +4943,7 @@
         <v>194</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D101" s="2" t="s">
         <v>54</v>
@@ -4936,7 +4970,7 @@
         <v>196</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D102" s="2" t="s">
         <v>54</v>
@@ -5088,13 +5122,13 @@
         <v>205</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D108" s="2" t="s">
         <v>109</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="F108" s="7" t="s">
         <v>6</v>
@@ -5140,7 +5174,7 @@
         <v>209</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D110" s="2" t="s">
         <v>141</v>
@@ -5192,7 +5226,7 @@
         <v>212</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D112" s="2" t="s">
         <v>54</v>
@@ -5294,7 +5328,7 @@
         <v>218</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D116" s="2" t="s">
         <v>54</v>
@@ -5371,7 +5405,7 @@
         <v>223</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D119" s="2" t="s">
         <v>109</v>
@@ -5398,7 +5432,7 @@
         <v>224</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D120" s="2" t="s">
         <v>141</v>
@@ -5425,13 +5459,13 @@
         <v>226</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="D121" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E121" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F121" s="7" t="s">
         <v>6</v>
@@ -5452,7 +5486,7 @@
         <v>106</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D122" s="2" t="s">
         <v>30</v>
@@ -5479,13 +5513,13 @@
         <v>229</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D123" s="2" t="s">
         <v>54</v>
       </c>
       <c r="E123" s="2" t="s">
-        <v>230</v>
+        <v>542</v>
       </c>
       <c r="F123" s="7" t="s">
         <v>6</v>
@@ -5503,10 +5537,10 @@
         <v>2017</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D124" s="2" t="s">
         <v>141</v>
@@ -5530,10 +5564,10 @@
         <v>2017</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D125" s="2" t="s">
         <v>54</v>
@@ -5557,7 +5591,7 @@
         <v>2017</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C126" s="2"/>
       <c r="D126" s="2" t="s">
@@ -5582,7 +5616,7 @@
         <v>2018</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C127" s="2"/>
       <c r="D127" s="2" t="s">
@@ -5607,10 +5641,10 @@
         <v>2018</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D128" s="2" t="s">
         <v>165</v>
@@ -5634,14 +5668,14 @@
         <v>2018</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C129" s="2"/>
       <c r="D129" s="2" t="s">
         <v>103</v>
       </c>
       <c r="E129" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F129" s="7" t="s">
         <v>7</v>
@@ -5659,10 +5693,10 @@
         <v>2018</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D130" s="2" t="s">
         <v>109</v>
@@ -5686,10 +5720,10 @@
         <v>2018</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D131" s="2" t="s">
         <v>54</v>
@@ -5713,14 +5747,14 @@
         <v>2018</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C132" s="2"/>
       <c r="D132" s="2" t="s">
         <v>141</v>
       </c>
       <c r="E132" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F132" s="7" t="s">
         <v>6</v>
@@ -5763,7 +5797,7 @@
         <v>2018</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C134" s="2"/>
       <c r="D134" s="2" t="s">
@@ -5788,14 +5822,14 @@
         <v>2018</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C135" s="2"/>
       <c r="D135" s="2" t="s">
         <v>154</v>
       </c>
       <c r="E135" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F135" s="7" t="s">
         <v>7</v>
@@ -5813,16 +5847,16 @@
         <v>2018</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D136" s="2" t="s">
         <v>141</v>
       </c>
       <c r="E136" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F136" s="7" t="s">
         <v>6</v>
@@ -5840,16 +5874,16 @@
         <v>2018</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D137" s="2" t="s">
         <v>54</v>
       </c>
       <c r="E137" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F137" s="7" t="s">
         <v>6</v>
@@ -5892,16 +5926,16 @@
         <v>2018</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D139" s="2" t="s">
         <v>25</v>
       </c>
       <c r="E139" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F139" s="7" t="s">
         <v>6</v>
@@ -5919,14 +5953,14 @@
         <v>2018</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C140" s="2"/>
       <c r="D140" s="2" t="s">
         <v>112</v>
       </c>
       <c r="E140" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F140" s="7" t="s">
         <v>7</v>
@@ -5944,14 +5978,14 @@
         <v>2018</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C141" s="2"/>
       <c r="D141" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E141" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F141" s="7" t="s">
         <v>6</v>
@@ -5969,14 +6003,14 @@
         <v>2018</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C142" s="2"/>
       <c r="D142" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E142" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F142" s="7" t="s">
         <v>6</v>
@@ -5994,10 +6028,10 @@
         <v>2018</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D143" s="2" t="s">
         <v>141</v>
@@ -6021,16 +6055,16 @@
         <v>2019</v>
       </c>
       <c r="B144" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="D144" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="C144" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="D144" s="2" t="s">
+      <c r="E144" s="2" t="s">
         <v>261</v>
-      </c>
-      <c r="E144" s="2" t="s">
-        <v>262</v>
       </c>
       <c r="F144" s="7" t="s">
         <v>6</v>
@@ -6048,7 +6082,7 @@
         <v>2019</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C145" s="2"/>
       <c r="D145" s="2" t="s">
@@ -6073,14 +6107,14 @@
         <v>2019</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C146" s="2"/>
       <c r="D146" s="2" t="s">
         <v>144</v>
       </c>
       <c r="E146" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F146" s="7" t="s">
         <v>6</v>
@@ -6126,7 +6160,7 @@
         <v>74</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D148" s="2" t="s">
         <v>30</v>
@@ -6153,7 +6187,7 @@
         <v>124</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D149" s="2" t="s">
         <v>30</v>
@@ -6180,7 +6214,7 @@
         <v>83</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D150" s="2" t="s">
         <v>30</v>
@@ -6204,14 +6238,14 @@
         <v>2019</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C151" s="2"/>
       <c r="D151" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E151" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F151" s="7" t="s">
         <v>6</v>
@@ -6229,14 +6263,14 @@
         <v>2019</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C152" s="2"/>
       <c r="D152" s="2" t="s">
         <v>141</v>
       </c>
       <c r="E152" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F152" s="7" t="s">
         <v>6</v>
@@ -6254,16 +6288,16 @@
         <v>2019</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="D153" s="2" t="s">
         <v>144</v>
       </c>
       <c r="E153" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F153" s="7" t="s">
         <v>6</v>
@@ -6281,7 +6315,7 @@
         <v>2019</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C154" s="2"/>
       <c r="D154" s="2" t="s">
@@ -6301,21 +6335,21 @@
       </c>
       <c r="I154" s="7"/>
     </row>
-    <row r="155" spans="1:9" s="5" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+    <row r="155" spans="1:9" s="5" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A155" s="7">
         <v>2020</v>
       </c>
       <c r="B155" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D155" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="C155" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="D155" s="2" t="s">
+      <c r="E155" s="2" t="s">
         <v>282</v>
-      </c>
-      <c r="E155" s="2" t="s">
-        <v>283</v>
       </c>
       <c r="F155" s="7" t="s">
         <v>6</v>
@@ -6336,7 +6370,7 @@
         <v>136</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D156" s="2" t="s">
         <v>30</v>
@@ -6360,14 +6394,14 @@
         <v>2020</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C157" s="2"/>
       <c r="D157" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E157" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F157" s="7" t="s">
         <v>6</v>
@@ -6385,7 +6419,7 @@
         <v>2020</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C158" s="2"/>
       <c r="D158" s="2" t="s">
@@ -6410,16 +6444,16 @@
         <v>2020</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D159" s="2" t="s">
         <v>54</v>
       </c>
       <c r="E159" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F159" s="7" t="s">
         <v>6</v>
@@ -6437,14 +6471,14 @@
         <v>2020</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C160" s="2"/>
       <c r="D160" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E160" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F160" s="7" t="s">
         <v>7</v>
@@ -6462,16 +6496,16 @@
         <v>2020</v>
       </c>
       <c r="B161" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="C161" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="D161" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="C161" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="D161" s="2" t="s">
-        <v>294</v>
-      </c>
       <c r="E161" s="2" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="F161" s="7" t="s">
         <v>6</v>
@@ -6489,14 +6523,14 @@
         <v>2020</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C162" s="2"/>
       <c r="D162" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E162" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F162" s="7" t="s">
         <v>6</v>
@@ -6514,7 +6548,7 @@
         <v>2020</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C163" s="2"/>
       <c r="D163" s="2" t="s">
@@ -6539,10 +6573,10 @@
         <v>2020</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D164" s="2" t="s">
         <v>38</v>
@@ -6566,7 +6600,7 @@
         <v>2020</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C165" s="2"/>
       <c r="D165" s="2" t="s">
@@ -6591,16 +6625,16 @@
         <v>2020</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D166" s="2" t="s">
         <v>54</v>
       </c>
       <c r="E166" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F166" s="7" t="s">
         <v>6</v>
@@ -6618,16 +6652,16 @@
         <v>2020</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D167" s="2" t="s">
         <v>54</v>
       </c>
       <c r="E167" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F167" s="7" t="s">
         <v>6</v>
@@ -6645,7 +6679,7 @@
         <v>2020</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C168" s="2"/>
       <c r="D168" s="2" t="s">
@@ -6670,16 +6704,16 @@
         <v>2020</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D169" s="2" t="s">
         <v>54</v>
       </c>
       <c r="E169" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F169" s="7" t="s">
         <v>6</v>
@@ -6697,16 +6731,16 @@
         <v>2020</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D170" s="2" t="s">
         <v>144</v>
       </c>
       <c r="E170" s="2" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="F170" s="7" t="s">
         <v>6</v>
@@ -6724,16 +6758,16 @@
         <v>2020</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D171" s="2" t="s">
         <v>54</v>
       </c>
       <c r="E171" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F171" s="7" t="s">
         <v>6</v>
@@ -6751,10 +6785,10 @@
         <v>2020</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D172" s="2" t="s">
         <v>54</v>
@@ -6778,14 +6812,14 @@
         <v>2020</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C173" s="2"/>
       <c r="D173" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E173" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F173" s="7" t="s">
         <v>6</v>
@@ -6803,16 +6837,16 @@
         <v>2020</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D174" s="2" t="s">
         <v>141</v>
       </c>
       <c r="E174" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F174" s="7" t="s">
         <v>6</v>
@@ -6830,16 +6864,16 @@
         <v>2020</v>
       </c>
       <c r="B175" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="C175" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="D175" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="E175" s="2" t="s">
         <v>315</v>
-      </c>
-      <c r="C175" s="2" t="s">
-        <v>444</v>
-      </c>
-      <c r="D175" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="E175" s="2" t="s">
-        <v>316</v>
       </c>
       <c r="F175" s="7" t="s">
         <v>6</v>
@@ -6857,16 +6891,16 @@
         <v>2021</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D176" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E176" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F176" s="7" t="s">
         <v>6</v>
@@ -6884,16 +6918,16 @@
         <v>2021</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D177" s="2" t="s">
         <v>54</v>
       </c>
       <c r="E177" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F177" s="7" t="s">
         <v>6</v>
@@ -6911,16 +6945,16 @@
         <v>2021</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D178" s="2" t="s">
         <v>141</v>
       </c>
       <c r="E178" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F178" s="7" t="s">
         <v>6</v>
@@ -6938,16 +6972,16 @@
         <v>2021</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D179" s="2" t="s">
         <v>109</v>
       </c>
       <c r="E179" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F179" s="7" t="s">
         <v>6</v>
@@ -6965,14 +6999,14 @@
         <v>2021</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C180" s="2"/>
       <c r="D180" s="2" t="s">
         <v>216</v>
       </c>
       <c r="E180" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F180" s="7" t="s">
         <v>6</v>
@@ -6990,16 +7024,16 @@
         <v>2021</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D181" s="2" t="s">
         <v>54</v>
       </c>
       <c r="E181" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F181" s="7" t="s">
         <v>6</v>
@@ -7017,7 +7051,7 @@
         <v>2021</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C182" s="2"/>
       <c r="D182" s="2" t="s">
@@ -7042,14 +7076,14 @@
         <v>2021</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C183" s="2"/>
       <c r="D183" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E183" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F183" s="7" t="s">
         <v>6</v>
@@ -7067,7 +7101,7 @@
         <v>2021</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C184" s="2"/>
       <c r="D184" s="2" t="s">
@@ -7092,16 +7126,16 @@
         <v>2021</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D185" s="2" t="s">
         <v>54</v>
       </c>
       <c r="E185" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F185" s="7" t="s">
         <v>6</v>
@@ -7119,7 +7153,7 @@
         <v>2021</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C186" s="2"/>
       <c r="D186" s="2" t="s">
@@ -7144,16 +7178,16 @@
         <v>2021</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D187" s="2" t="s">
         <v>141</v>
       </c>
       <c r="E187" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="F187" s="7" t="s">
         <v>6</v>
@@ -7171,16 +7205,16 @@
         <v>2021</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D188" s="2" t="s">
         <v>54</v>
       </c>
       <c r="E188" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F188" s="7" t="s">
         <v>6</v>
@@ -7198,14 +7232,14 @@
         <v>2021</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C189" s="2"/>
       <c r="D189" s="2" t="s">
         <v>144</v>
       </c>
       <c r="E189" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F189" s="7" t="s">
         <v>6</v>
@@ -7226,7 +7260,7 @@
         <v>138</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D190" s="2" t="s">
         <v>30</v>
@@ -7250,16 +7284,16 @@
         <v>2021</v>
       </c>
       <c r="B191" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="C191" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="D191" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="C191" s="2" t="s">
-        <v>435</v>
-      </c>
-      <c r="D191" s="2" t="s">
+      <c r="E191" s="2" t="s">
         <v>343</v>
-      </c>
-      <c r="E191" s="2" t="s">
-        <v>344</v>
       </c>
       <c r="F191" s="7" t="s">
         <v>6</v>
@@ -7277,16 +7311,16 @@
         <v>2018</v>
       </c>
       <c r="B192" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C192" s="2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D192" s="2" t="s">
         <v>54</v>
       </c>
       <c r="E192" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F192" s="7" t="s">
         <v>6</v>
@@ -7304,16 +7338,16 @@
         <v>2022</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D193" s="2" t="s">
         <v>141</v>
       </c>
       <c r="E193" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="F193" s="7" t="s">
         <v>6</v>
@@ -7331,14 +7365,14 @@
         <v>2022</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C194" s="2"/>
       <c r="D194" s="2" t="s">
         <v>216</v>
       </c>
       <c r="E194" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F194" s="7" t="s">
         <v>6</v>
@@ -7356,16 +7390,16 @@
         <v>2022</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D195" s="2" t="s">
         <v>54</v>
       </c>
       <c r="E195" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F195" s="7" t="s">
         <v>6</v>
@@ -7383,16 +7417,16 @@
         <v>2022</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C196" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D196" s="2" t="s">
         <v>144</v>
       </c>
       <c r="E196" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F196" s="7" t="s">
         <v>6</v>
@@ -7410,14 +7444,14 @@
         <v>2022</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C197" s="2"/>
       <c r="D197" s="2" t="s">
         <v>160</v>
       </c>
       <c r="E197" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F197" s="7" t="s">
         <v>6</v>
@@ -7435,14 +7469,14 @@
         <v>2022</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C198" s="2"/>
       <c r="D198" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="E198" s="2" t="s">
         <v>362</v>
-      </c>
-      <c r="E198" s="2" t="s">
-        <v>363</v>
       </c>
       <c r="F198" s="7" t="s">
         <v>6</v>
@@ -7460,14 +7494,14 @@
         <v>2022</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="C199" s="2"/>
       <c r="D199" s="2" t="s">
         <v>109</v>
       </c>
       <c r="E199" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F199" s="7" t="s">
         <v>6</v>
@@ -7485,16 +7519,16 @@
         <v>2022</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D200" s="2" t="s">
         <v>141</v>
       </c>
       <c r="E200" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F200" s="7" t="s">
         <v>6</v>
@@ -7512,16 +7546,16 @@
         <v>2022</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C201" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D201" s="2" t="s">
         <v>154</v>
       </c>
       <c r="E201" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F201" s="7" t="s">
         <v>6</v>
@@ -7539,16 +7573,16 @@
         <v>2022</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C202" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D202" s="2" t="s">
         <v>160</v>
       </c>
       <c r="E202" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F202" s="7" t="s">
         <v>6</v>
@@ -7566,14 +7600,14 @@
         <v>2022</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C203" s="2"/>
       <c r="D203" s="2" t="s">
         <v>160</v>
       </c>
       <c r="E203" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F203" s="7" t="s">
         <v>6</v>
@@ -7591,7 +7625,7 @@
         <v>2022</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C204" s="2"/>
       <c r="D204" s="2" t="s">
@@ -7616,16 +7650,16 @@
         <v>2023</v>
       </c>
       <c r="B205" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C205" s="2" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D205" s="2" t="s">
         <v>54</v>
       </c>
       <c r="E205" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F205" s="7" t="s">
         <v>6</v>
@@ -7643,10 +7677,10 @@
         <v>2023</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C206" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D206" s="2" t="s">
         <v>25</v>
@@ -7670,14 +7704,14 @@
         <v>2023</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C207" s="2"/>
       <c r="D207" s="2" t="s">
         <v>160</v>
       </c>
       <c r="E207" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F207" s="7" t="s">
         <v>6</v>
@@ -7695,14 +7729,14 @@
         <v>2023</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C208" s="2"/>
       <c r="D208" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="E208" s="2" t="s">
         <v>370</v>
-      </c>
-      <c r="E208" s="2" t="s">
-        <v>371</v>
       </c>
       <c r="F208" s="7" t="s">
         <v>6</v>
@@ -7720,14 +7754,14 @@
         <v>2023</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C209" s="2"/>
       <c r="D209" s="2" t="s">
         <v>160</v>
       </c>
       <c r="E209" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F209" s="7" t="s">
         <v>6</v>
@@ -7745,7 +7779,7 @@
         <v>2023</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C210" s="2"/>
       <c r="D210" s="2" t="s">
@@ -7770,14 +7804,14 @@
         <v>2023</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C211" s="2"/>
       <c r="D211" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E211" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F211" s="7" t="s">
         <v>6</v>
@@ -7795,7 +7829,7 @@
         <v>2023</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C212" s="2"/>
       <c r="D212" s="2" t="s">
@@ -7820,16 +7854,16 @@
         <v>2023</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C213" s="2" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D213" s="2" t="s">
         <v>141</v>
       </c>
       <c r="E213" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F213" s="7" t="s">
         <v>6</v>
@@ -7872,7 +7906,7 @@
         <v>2023</v>
       </c>
       <c r="B215" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C215" s="2"/>
       <c r="D215" s="2" t="s">
@@ -7897,14 +7931,14 @@
         <v>2023</v>
       </c>
       <c r="B216" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C216" s="2"/>
       <c r="D216" s="2" t="s">
         <v>160</v>
       </c>
       <c r="E216" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F216" s="7" t="s">
         <v>6</v>
@@ -7922,14 +7956,14 @@
         <v>2023</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C217" s="2"/>
       <c r="D217" s="2" t="s">
         <v>109</v>
       </c>
       <c r="E217" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F217" s="7" t="s">
         <v>6</v>
@@ -7947,14 +7981,14 @@
         <v>2023</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C218" s="2"/>
       <c r="D218" s="2" t="s">
         <v>141</v>
       </c>
       <c r="E218" s="2" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F218" s="7" t="s">
         <v>6</v>
@@ -7972,13 +8006,13 @@
         <v>2024</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D219" s="2" t="s">
         <v>35</v>
       </c>
       <c r="E219" s="2" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F219" s="7" t="s">
         <v>6</v>
@@ -7995,14 +8029,14 @@
         <v>2024</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>464</v>
-      </c>
-      <c r="C220" s="14"/>
+        <v>463</v>
+      </c>
+      <c r="C220" s="13"/>
       <c r="D220" s="2" t="s">
         <v>35</v>
       </c>
       <c r="E220" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F220" s="7" t="s">
         <v>6</v>
@@ -8019,16 +8053,16 @@
         <v>2024</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C221" s="2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D221" s="2" t="s">
         <v>54</v>
       </c>
       <c r="E221" s="2" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="F221" s="7" t="s">
         <v>6</v>
@@ -8045,14 +8079,14 @@
         <v>2024</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C222" s="2"/>
       <c r="D222" s="2" t="s">
         <v>160</v>
       </c>
       <c r="E222" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="F222" s="7" t="s">
         <v>6</v>
@@ -8069,14 +8103,14 @@
         <v>2024</v>
       </c>
       <c r="B223" s="2" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C223" s="2"/>
       <c r="D223" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="E223" s="2" t="s">
         <v>468</v>
-      </c>
-      <c r="E223" s="2" t="s">
-        <v>469</v>
       </c>
       <c r="F223" s="7" t="s">
         <v>6</v>
@@ -8093,16 +8127,16 @@
         <v>2024</v>
       </c>
       <c r="B224" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="C224" s="2" t="s">
         <v>471</v>
       </c>
-      <c r="C224" s="2" t="s">
+      <c r="D224" s="2" t="s">
         <v>472</v>
       </c>
-      <c r="D224" s="2" t="s">
+      <c r="E224" s="2" t="s">
         <v>473</v>
-      </c>
-      <c r="E224" s="2" t="s">
-        <v>474</v>
       </c>
       <c r="F224" s="2" t="s">
         <v>6</v>
@@ -8119,16 +8153,16 @@
         <v>2024</v>
       </c>
       <c r="B225" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C225" s="2" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D225" s="2" t="s">
         <v>141</v>
       </c>
       <c r="E225" s="2" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="F225" s="2" t="s">
         <v>6</v>
@@ -8145,16 +8179,16 @@
         <v>2024</v>
       </c>
       <c r="B226" s="2" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C226" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D226" s="2" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="E226" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="F226" s="7" t="s">
         <v>6</v>
@@ -8172,16 +8206,16 @@
         <v>2024</v>
       </c>
       <c r="B227" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="C227" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="D227" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="E227" s="2" t="s">
         <v>484</v>
-      </c>
-      <c r="C227" s="2" t="s">
-        <v>489</v>
-      </c>
-      <c r="D227" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="E227" s="2" t="s">
-        <v>485</v>
       </c>
       <c r="F227" s="7" t="s">
         <v>6</v>
@@ -8198,16 +8232,16 @@
         <v>2024</v>
       </c>
       <c r="B228" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="C228" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="D228" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="E228" s="2" t="s">
         <v>480</v>
-      </c>
-      <c r="C228" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="D228" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="E228" s="2" t="s">
-        <v>481</v>
       </c>
       <c r="F228" s="7" t="s">
         <v>6</v>
@@ -8224,16 +8258,16 @@
         <v>2024</v>
       </c>
       <c r="B229" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C229" s="2" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D229" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E229" s="2" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="F229" s="7" t="s">
         <v>6</v>
@@ -8250,14 +8284,14 @@
         <v>2024</v>
       </c>
       <c r="B230" s="2" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C230" s="2"/>
       <c r="D230" s="2" t="s">
         <v>216</v>
       </c>
       <c r="E230" s="2" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="F230" s="7" t="s">
         <v>6</v>
@@ -8274,16 +8308,16 @@
         <v>2024</v>
       </c>
       <c r="B231" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="C231" s="2" t="s">
         <v>497</v>
-      </c>
-      <c r="C231" s="2" t="s">
-        <v>498</v>
       </c>
       <c r="D231" s="2" t="s">
         <v>141</v>
       </c>
       <c r="E231" s="2" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="F231" s="7" t="s">
         <v>6</v>
@@ -8300,10 +8334,10 @@
         <v>2024</v>
       </c>
       <c r="B232" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C232" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D232" s="2" t="s">
         <v>38</v>
@@ -8326,16 +8360,16 @@
         <v>2024</v>
       </c>
       <c r="B233" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="C233" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="C233" s="2" t="s">
-        <v>501</v>
-      </c>
-      <c r="D233" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E233" s="2" t="s">
-        <v>504</v>
+      <c r="D233" s="14" t="s">
+        <v>532</v>
+      </c>
+      <c r="E233" s="14" t="s">
+        <v>533</v>
       </c>
       <c r="F233" s="7" t="s">
         <v>6</v>
@@ -8352,13 +8386,13 @@
         <v>2024</v>
       </c>
       <c r="B234" s="2" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D234" s="2" t="s">
         <v>109</v>
       </c>
       <c r="E234" s="2" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="F234" s="7" t="s">
         <v>6</v>
@@ -8375,10 +8409,10 @@
         <v>2024</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C235" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D235" s="2" t="s">
         <v>30</v>
@@ -8401,208 +8435,311 @@
         <v>2025</v>
       </c>
       <c r="B236" s="2" t="s">
+        <v>512</v>
+      </c>
+      <c r="C236" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="D236" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="E236" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="F236" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G236" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H236" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="237" spans="1:9" ht="29" x14ac:dyDescent="0.2">
+      <c r="A237" s="5">
+        <v>2025</v>
+      </c>
+      <c r="B237" s="14" t="s">
+        <v>513</v>
+      </c>
+      <c r="C237" s="14" t="s">
+        <v>530</v>
+      </c>
+      <c r="D237" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="E237" s="14" t="s">
+        <v>518</v>
+      </c>
+      <c r="F237" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G237" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H237" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="238" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A238" s="5">
+        <v>2025</v>
+      </c>
+      <c r="B238" s="14" t="s">
         <v>514</v>
       </c>
-      <c r="C236" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="D236" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="E236" s="2" t="s">
-        <v>481</v>
-      </c>
-      <c r="F236" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G236" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="H236" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="237" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A237" s="7">
+      <c r="C238" s="14" t="s">
+        <v>412</v>
+      </c>
+      <c r="D238" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E238" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="F238" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G238" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H238" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="239" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A239" s="5">
         <v>2025</v>
       </c>
-      <c r="B237" s="2" t="s">
-        <v>515</v>
-      </c>
-      <c r="C237" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="D237" s="2" t="s">
+      <c r="B239" s="14" t="s">
+        <v>516</v>
+      </c>
+      <c r="C239" s="12"/>
+      <c r="D239" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E239" s="14" t="s">
+        <v>517</v>
+      </c>
+      <c r="F239" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G239" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H239" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="240" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A240" s="5">
+        <v>2025</v>
+      </c>
+      <c r="B240" s="14" t="s">
+        <v>527</v>
+      </c>
+      <c r="C240" s="12"/>
+      <c r="D240" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="E240" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="F240" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G240" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H240" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="241" spans="1:9" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.2">
+      <c r="A241" s="5">
+        <v>2025</v>
+      </c>
+      <c r="B241" s="14" t="s">
+        <v>520</v>
+      </c>
+      <c r="C241" s="14" t="s">
+        <v>522</v>
+      </c>
+      <c r="D241" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="E241" s="14" t="s">
+        <v>521</v>
+      </c>
+      <c r="F241" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G241" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H241" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="242" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A242" s="5">
+        <v>2025</v>
+      </c>
+      <c r="B242" s="14" t="s">
+        <v>529</v>
+      </c>
+      <c r="C242" s="14" t="s">
+        <v>528</v>
+      </c>
+      <c r="D242" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="E237" s="2" t="s">
-        <v>520</v>
-      </c>
-      <c r="F237" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G237" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="H237" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="238" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A238" s="7">
+      <c r="E242" s="14" t="s">
+        <v>523</v>
+      </c>
+      <c r="F242" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G242" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H242" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="243" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A243" s="5">
         <v>2025</v>
       </c>
-      <c r="B238" s="2" t="s">
-        <v>516</v>
-      </c>
-      <c r="C238" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D238" s="2" t="s">
+      <c r="B243" s="14" t="s">
+        <v>524</v>
+      </c>
+      <c r="C243" s="14" t="s">
+        <v>526</v>
+      </c>
+      <c r="D243" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E238" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="F238" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G238" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="H238" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="239" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A239" s="7">
+      <c r="E243" s="14" t="s">
+        <v>525</v>
+      </c>
+      <c r="F243" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G243" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H243" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="244" spans="1:9" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A244" s="5">
         <v>2025</v>
       </c>
-      <c r="B239" s="2" t="s">
-        <v>518</v>
-      </c>
-      <c r="D239" s="2" t="s">
+      <c r="B244" s="14" t="s">
+        <v>531</v>
+      </c>
+      <c r="C244" s="14"/>
+      <c r="D244" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="E244" s="14" t="s">
+        <v>354</v>
+      </c>
+      <c r="F244" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G244" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H244" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="245" spans="1:9" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A245" s="5">
+        <v>2025</v>
+      </c>
+      <c r="B245" s="5" t="s">
+        <v>534</v>
+      </c>
+      <c r="C245" s="5" t="s">
+        <v>389</v>
+      </c>
+      <c r="D245" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E239" s="2" t="s">
-        <v>519</v>
-      </c>
-      <c r="F239" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G239" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="H239" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="240" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A240" s="7">
+      <c r="E245" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F245" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G245" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H245" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="246" spans="1:9" ht="43" x14ac:dyDescent="0.2">
+      <c r="A246" s="5">
         <v>2025</v>
       </c>
-      <c r="B240" s="10" t="s">
-        <v>529</v>
-      </c>
-      <c r="C240" s="12"/>
-      <c r="D240" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="E240" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="F240" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G240" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="H240" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="241" spans="1:8" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.2">
-      <c r="A241" s="4">
+      <c r="B246" s="5" t="s">
+        <v>535</v>
+      </c>
+      <c r="C246" s="14" t="s">
+        <v>537</v>
+      </c>
+      <c r="D246" s="5" t="s">
+        <v>536</v>
+      </c>
+      <c r="E246" s="5" t="s">
+        <v>538</v>
+      </c>
+      <c r="F246" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G246" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H246" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I246" s="6"/>
+    </row>
+    <row r="247" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A247" s="5">
         <v>2025</v>
       </c>
-      <c r="B241" s="10" t="s">
-        <v>522</v>
-      </c>
-      <c r="C241" s="10" t="s">
-        <v>524</v>
-      </c>
-      <c r="D241" s="10" t="s">
-        <v>165</v>
-      </c>
-      <c r="E241" s="10" t="s">
-        <v>523</v>
-      </c>
-      <c r="F241" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G241" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H241" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="242" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A242" s="4">
-        <v>2025</v>
-      </c>
-      <c r="B242" s="10" t="s">
-        <v>531</v>
-      </c>
-      <c r="C242" s="10" t="s">
-        <v>530</v>
-      </c>
-      <c r="D242" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="E242" s="10" t="s">
-        <v>525</v>
-      </c>
-      <c r="F242" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G242" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H242" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="243" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A243" s="4">
-        <v>2025</v>
-      </c>
-      <c r="B243" s="10" t="s">
-        <v>526</v>
-      </c>
-      <c r="C243" s="10" t="s">
-        <v>528</v>
-      </c>
-      <c r="D243" s="10" t="s">
+      <c r="B247" s="5" t="s">
+        <v>539</v>
+      </c>
+      <c r="C247" s="5" t="s">
+        <v>540</v>
+      </c>
+      <c r="D247" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E243" s="10" t="s">
-        <v>527</v>
-      </c>
-      <c r="F243" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G243" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H243" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="244" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E244" s="2"/>
+      <c r="E247" s="5" t="s">
+        <v>541</v>
+      </c>
+      <c r="F247" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G247" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H247" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I247" s="6"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I247" xr:uid="{6B89377A-76F6-CA40-8081-AAD80BFAB6B8}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H217">
     <sortCondition ref="B2:B217"/>
   </sortState>
@@ -8626,37 +8763,37 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="59" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="45" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add news for 5.1 (#1233)
</commit_message>
<xml_diff>
--- a/src/main/webapp/content/files/oncologyTherapies/fda_approved_oncology_therapies.xlsx
+++ b/src/main/webapp/content/files/oncologyTherapies/fda_approved_oncology_therapies.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mskcc-my.sharepoint.com/personal/phillis2_mskcc_org/Documents/Precision Oncology Drug Page for Website/FDA-Approved_Oncology_therapies_bi_monthly updates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cavendk1/Documents/New onc therapies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{8C0F3825-168A-3C4C-913E-753BB014F271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33F0D526-34CA-1149-A4CE-440D95A17625}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59E48DA2-5F66-174E-9D87-A0BE250055A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="49820" yWindow="2800" windowWidth="29560" windowHeight="16900" xr2:uid="{D862B214-800F-AF40-9BAA-60FE1781D5C8}"/>
+    <workbookView xWindow="3480" yWindow="-21100" windowWidth="30240" windowHeight="17460" xr2:uid="{D862B214-800F-AF40-9BAA-60FE1781D5C8}"/>
   </bookViews>
   <sheets>
     <sheet name="FDA-Approved Oncology Therapies" sheetId="1" r:id="rId1"/>
     <sheet name="Footnotes" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'FDA-Approved Oncology Therapies'!$A$1:$H$243</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'FDA-Approved Oncology Therapies'!$A$1:$I$247</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1595" uniqueCount="532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1622" uniqueCount="543">
   <si>
     <t>Year of drug’s first FDA- approval</t>
   </si>
@@ -728,9 +728,6 @@
   </si>
   <si>
     <t>Neratinib</t>
-  </si>
-  <si>
-    <t>EGFR//HER2 (ERBB2)/HER4 (ERBB4) inhibitor</t>
   </si>
   <si>
     <t>Niraparib</t>
@@ -1708,9 +1705,6 @@
     <t>dMMR</t>
   </si>
   <si>
-    <t>Bispecific HER2/HER3-directed T-cell engager</t>
-  </si>
-  <si>
     <t>Menin inhibitor</t>
   </si>
   <si>
@@ -1845,6 +1839,46 @@
   </si>
   <si>
     <t>Telisotuzumab</t>
+  </si>
+  <si>
+    <t>*HR+/HER2-
+*EGFR Oncogenic Mutations</t>
+  </si>
+  <si>
+    <t>Linvoseltamab</t>
+  </si>
+  <si>
+    <t>Bispecific antibody</t>
+  </si>
+  <si>
+    <t>Bispecific HER2/HER3 antibody</t>
+  </si>
+  <si>
+    <t>Sunvozertinib</t>
+  </si>
+  <si>
+    <t>Dordaviprone</t>
+  </si>
+  <si>
+    <t>Protease activator</t>
+  </si>
+  <si>
+    <t>H3 K27M (K28M): H3-3A (H3F3A), H3C2 (HIST1H3B), H3C3 (HIST1H3C)</t>
+  </si>
+  <si>
+    <t>DRD2 and ClpP agonist</t>
+  </si>
+  <si>
+    <t>Zongertinib</t>
+  </si>
+  <si>
+    <t>ERBB2 TKD activating mutations</t>
+  </si>
+  <si>
+    <t>HER2 (ERBB2) inhibitor</t>
+  </si>
+  <si>
+    <t>EGFR/HER2 (ERBB2)/HER4 (ERBB4) inhibitor</t>
   </si>
 </sst>
 </file>
@@ -1977,9 +2011,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1990,6 +2021,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2010,9 +2044,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2050,7 +2084,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2156,7 +2190,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2298,7 +2332,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2306,38 +2340,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B89377A-76F6-CA40-8081-AAD80BFAB6B8}">
-  <dimension ref="A1:I244"/>
+  <dimension ref="A1:I247"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A235" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B173" sqref="B173"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A230" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C245" sqref="C245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.1640625" customWidth="1"/>
-    <col min="2" max="2" width="26.1640625" style="12" customWidth="1"/>
-    <col min="3" max="3" width="27.83203125" style="12" customWidth="1"/>
-    <col min="4" max="4" width="29.5" style="12" customWidth="1"/>
-    <col min="5" max="5" width="77" style="12" customWidth="1"/>
+    <col min="2" max="2" width="26.1640625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" style="11" customWidth="1"/>
+    <col min="4" max="4" width="29.5" style="11" customWidth="1"/>
+    <col min="5" max="5" width="77" style="11" customWidth="1"/>
     <col min="10" max="16384" width="11.1640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="13" customFormat="1" ht="47" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="12" customFormat="1" ht="47" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>504</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>505</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>506</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="E1" s="8" t="s">
         <v>507</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>508</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>509</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>1</v>
@@ -2346,9 +2380,9 @@
         <v>2</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>477</v>
-      </c>
-      <c r="I1" s="12"/>
+        <v>476</v>
+      </c>
+      <c r="I1" s="11"/>
     </row>
     <row r="2" spans="1:9" s="5" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
@@ -2408,7 +2442,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>13</v>
@@ -2485,7 +2519,7 @@
         <v>19</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>20</v>
@@ -2537,7 +2571,7 @@
         <v>24</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>25</v>
@@ -2564,7 +2598,7 @@
         <v>27</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>20</v>
@@ -2588,16 +2622,16 @@
         <v>2018</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>54</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>6</v>
@@ -2668,7 +2702,7 @@
         <v>37</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>38</v>
@@ -2699,7 +2733,7 @@
         <v>25</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>6</v>
@@ -2745,7 +2779,7 @@
         <v>43</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>25</v>
@@ -2872,7 +2906,7 @@
         <v>53</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>54</v>
@@ -2899,7 +2933,7 @@
         <v>56</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>20</v>
@@ -2976,7 +3010,7 @@
         <v>60</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>38</v>
@@ -3028,7 +3062,7 @@
         <v>63</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>54</v>
@@ -3105,7 +3139,7 @@
         <v>29</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>30</v>
@@ -3129,14 +3163,14 @@
         <v>2019</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F32" s="7" t="s">
         <v>6</v>
@@ -3207,7 +3241,7 @@
         <v>73</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>38</v>
@@ -3231,16 +3265,16 @@
         <v>2019</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>54</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F36" s="7" t="s">
         <v>6</v>
@@ -3311,7 +3345,7 @@
         <v>81</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>54</v>
@@ -3338,7 +3372,7 @@
         <v>227</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>30</v>
@@ -3432,7 +3466,7 @@
       </c>
       <c r="I43" s="7"/>
     </row>
-    <row r="44" spans="1:9" s="5" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:9" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A44" s="7">
         <v>2009</v>
       </c>
@@ -3440,7 +3474,7 @@
         <v>90</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>86</v>
@@ -3489,14 +3523,14 @@
         <v>2019</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F46" s="7" t="s">
         <v>6</v>
@@ -3689,10 +3723,10 @@
         <v>2011</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>20</v>
@@ -3716,16 +3750,16 @@
         <v>2020</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>54</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F55" s="7" t="s">
         <v>6</v>
@@ -3818,16 +3852,16 @@
         <v>2019</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>54</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F59" s="7" t="s">
         <v>6</v>
@@ -3848,7 +3882,7 @@
         <v>118</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>54</v>
@@ -3922,14 +3956,14 @@
         <v>2021</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F63" s="7" t="s">
         <v>6</v>
@@ -3947,16 +3981,16 @@
         <v>2023</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>54</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="F64" s="7" t="s">
         <v>6</v>
@@ -4052,7 +4086,7 @@
         <v>133</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>134</v>
@@ -4071,7 +4105,7 @@
       </c>
       <c r="I68" s="7"/>
     </row>
-    <row r="69" spans="1:9" s="5" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:9" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A69" s="7">
         <v>2006</v>
       </c>
@@ -4079,7 +4113,7 @@
         <v>69</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>30</v>
@@ -4156,7 +4190,7 @@
         <v>143</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>144</v>
@@ -4183,7 +4217,7 @@
         <v>146</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>54</v>
@@ -4210,7 +4244,7 @@
         <v>147</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>54</v>
@@ -4237,7 +4271,7 @@
         <v>148</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>54</v>
@@ -4339,7 +4373,7 @@
         <v>156</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>54</v>
@@ -4391,7 +4425,7 @@
         <v>159</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>160</v>
@@ -4418,7 +4452,7 @@
         <v>162</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>54</v>
@@ -4445,7 +4479,7 @@
         <v>164</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>165</v>
@@ -4547,7 +4581,7 @@
         <v>173</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>109</v>
@@ -4574,7 +4608,7 @@
         <v>175</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>141</v>
@@ -4601,7 +4635,7 @@
         <v>177</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>109</v>
@@ -4678,7 +4712,7 @@
         <v>182</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>54</v>
@@ -4702,10 +4736,10 @@
         <v>2015</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>165</v>
@@ -4736,7 +4770,7 @@
         <v>20</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F94" s="7" t="s">
         <v>6</v>
@@ -4807,7 +4841,7 @@
         <v>188</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D97" s="2" t="s">
         <v>109</v>
@@ -4856,14 +4890,14 @@
         <v>2021</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C99" s="2"/>
       <c r="D99" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F99" s="7" t="s">
         <v>6</v>
@@ -4909,7 +4943,7 @@
         <v>194</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D101" s="2" t="s">
         <v>54</v>
@@ -4936,7 +4970,7 @@
         <v>196</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D102" s="2" t="s">
         <v>54</v>
@@ -5088,13 +5122,13 @@
         <v>205</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D108" s="2" t="s">
         <v>109</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="F108" s="7" t="s">
         <v>6</v>
@@ -5140,7 +5174,7 @@
         <v>209</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D110" s="2" t="s">
         <v>141</v>
@@ -5192,7 +5226,7 @@
         <v>212</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D112" s="2" t="s">
         <v>54</v>
@@ -5294,7 +5328,7 @@
         <v>218</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D116" s="2" t="s">
         <v>54</v>
@@ -5371,7 +5405,7 @@
         <v>223</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D119" s="2" t="s">
         <v>109</v>
@@ -5398,7 +5432,7 @@
         <v>224</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D120" s="2" t="s">
         <v>141</v>
@@ -5425,13 +5459,13 @@
         <v>226</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="D121" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E121" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F121" s="7" t="s">
         <v>6</v>
@@ -5452,7 +5486,7 @@
         <v>106</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D122" s="2" t="s">
         <v>30</v>
@@ -5479,13 +5513,13 @@
         <v>229</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D123" s="2" t="s">
         <v>54</v>
       </c>
       <c r="E123" s="2" t="s">
-        <v>230</v>
+        <v>542</v>
       </c>
       <c r="F123" s="7" t="s">
         <v>6</v>
@@ -5503,10 +5537,10 @@
         <v>2017</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D124" s="2" t="s">
         <v>141</v>
@@ -5530,10 +5564,10 @@
         <v>2017</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D125" s="2" t="s">
         <v>54</v>
@@ -5557,7 +5591,7 @@
         <v>2017</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C126" s="2"/>
       <c r="D126" s="2" t="s">
@@ -5582,7 +5616,7 @@
         <v>2018</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C127" s="2"/>
       <c r="D127" s="2" t="s">
@@ -5607,10 +5641,10 @@
         <v>2018</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D128" s="2" t="s">
         <v>165</v>
@@ -5634,14 +5668,14 @@
         <v>2018</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C129" s="2"/>
       <c r="D129" s="2" t="s">
         <v>103</v>
       </c>
       <c r="E129" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F129" s="7" t="s">
         <v>7</v>
@@ -5659,10 +5693,10 @@
         <v>2018</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D130" s="2" t="s">
         <v>109</v>
@@ -5686,10 +5720,10 @@
         <v>2018</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D131" s="2" t="s">
         <v>54</v>
@@ -5713,14 +5747,14 @@
         <v>2018</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C132" s="2"/>
       <c r="D132" s="2" t="s">
         <v>141</v>
       </c>
       <c r="E132" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F132" s="7" t="s">
         <v>6</v>
@@ -5763,7 +5797,7 @@
         <v>2018</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C134" s="2"/>
       <c r="D134" s="2" t="s">
@@ -5788,14 +5822,14 @@
         <v>2018</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C135" s="2"/>
       <c r="D135" s="2" t="s">
         <v>154</v>
       </c>
       <c r="E135" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F135" s="7" t="s">
         <v>7</v>
@@ -5813,16 +5847,16 @@
         <v>2018</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D136" s="2" t="s">
         <v>141</v>
       </c>
       <c r="E136" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F136" s="7" t="s">
         <v>6</v>
@@ -5840,16 +5874,16 @@
         <v>2018</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D137" s="2" t="s">
         <v>54</v>
       </c>
       <c r="E137" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F137" s="7" t="s">
         <v>6</v>
@@ -5892,16 +5926,16 @@
         <v>2018</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D139" s="2" t="s">
         <v>25</v>
       </c>
       <c r="E139" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F139" s="7" t="s">
         <v>6</v>
@@ -5919,14 +5953,14 @@
         <v>2018</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C140" s="2"/>
       <c r="D140" s="2" t="s">
         <v>112</v>
       </c>
       <c r="E140" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F140" s="7" t="s">
         <v>7</v>
@@ -5944,14 +5978,14 @@
         <v>2018</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C141" s="2"/>
       <c r="D141" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E141" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F141" s="7" t="s">
         <v>6</v>
@@ -5969,14 +6003,14 @@
         <v>2018</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C142" s="2"/>
       <c r="D142" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E142" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F142" s="7" t="s">
         <v>6</v>
@@ -5994,10 +6028,10 @@
         <v>2018</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D143" s="2" t="s">
         <v>141</v>
@@ -6021,16 +6055,16 @@
         <v>2019</v>
       </c>
       <c r="B144" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="D144" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="C144" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="D144" s="2" t="s">
+      <c r="E144" s="2" t="s">
         <v>261</v>
-      </c>
-      <c r="E144" s="2" t="s">
-        <v>262</v>
       </c>
       <c r="F144" s="7" t="s">
         <v>6</v>
@@ -6048,7 +6082,7 @@
         <v>2019</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C145" s="2"/>
       <c r="D145" s="2" t="s">
@@ -6073,14 +6107,14 @@
         <v>2019</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C146" s="2"/>
       <c r="D146" s="2" t="s">
         <v>144</v>
       </c>
       <c r="E146" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F146" s="7" t="s">
         <v>6</v>
@@ -6126,7 +6160,7 @@
         <v>74</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D148" s="2" t="s">
         <v>30</v>
@@ -6153,7 +6187,7 @@
         <v>124</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D149" s="2" t="s">
         <v>30</v>
@@ -6180,7 +6214,7 @@
         <v>83</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D150" s="2" t="s">
         <v>30</v>
@@ -6204,14 +6238,14 @@
         <v>2019</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C151" s="2"/>
       <c r="D151" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E151" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F151" s="7" t="s">
         <v>6</v>
@@ -6229,14 +6263,14 @@
         <v>2019</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C152" s="2"/>
       <c r="D152" s="2" t="s">
         <v>141</v>
       </c>
       <c r="E152" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F152" s="7" t="s">
         <v>6</v>
@@ -6254,16 +6288,16 @@
         <v>2019</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="D153" s="2" t="s">
         <v>144</v>
       </c>
       <c r="E153" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F153" s="7" t="s">
         <v>6</v>
@@ -6281,7 +6315,7 @@
         <v>2019</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C154" s="2"/>
       <c r="D154" s="2" t="s">
@@ -6301,21 +6335,21 @@
       </c>
       <c r="I154" s="7"/>
     </row>
-    <row r="155" spans="1:9" s="5" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+    <row r="155" spans="1:9" s="5" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A155" s="7">
         <v>2020</v>
       </c>
       <c r="B155" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D155" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="C155" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="D155" s="2" t="s">
+      <c r="E155" s="2" t="s">
         <v>282</v>
-      </c>
-      <c r="E155" s="2" t="s">
-        <v>283</v>
       </c>
       <c r="F155" s="7" t="s">
         <v>6</v>
@@ -6336,7 +6370,7 @@
         <v>136</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D156" s="2" t="s">
         <v>30</v>
@@ -6360,14 +6394,14 @@
         <v>2020</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C157" s="2"/>
       <c r="D157" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E157" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F157" s="7" t="s">
         <v>6</v>
@@ -6385,7 +6419,7 @@
         <v>2020</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C158" s="2"/>
       <c r="D158" s="2" t="s">
@@ -6410,16 +6444,16 @@
         <v>2020</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D159" s="2" t="s">
         <v>54</v>
       </c>
       <c r="E159" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F159" s="7" t="s">
         <v>6</v>
@@ -6437,14 +6471,14 @@
         <v>2020</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C160" s="2"/>
       <c r="D160" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E160" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F160" s="7" t="s">
         <v>7</v>
@@ -6462,16 +6496,16 @@
         <v>2020</v>
       </c>
       <c r="B161" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="C161" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="D161" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="C161" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="D161" s="2" t="s">
-        <v>294</v>
-      </c>
       <c r="E161" s="2" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="F161" s="7" t="s">
         <v>6</v>
@@ -6489,14 +6523,14 @@
         <v>2020</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C162" s="2"/>
       <c r="D162" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E162" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F162" s="7" t="s">
         <v>6</v>
@@ -6514,7 +6548,7 @@
         <v>2020</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C163" s="2"/>
       <c r="D163" s="2" t="s">
@@ -6539,10 +6573,10 @@
         <v>2020</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D164" s="2" t="s">
         <v>38</v>
@@ -6566,7 +6600,7 @@
         <v>2020</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C165" s="2"/>
       <c r="D165" s="2" t="s">
@@ -6591,16 +6625,16 @@
         <v>2020</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D166" s="2" t="s">
         <v>54</v>
       </c>
       <c r="E166" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F166" s="7" t="s">
         <v>6</v>
@@ -6618,16 +6652,16 @@
         <v>2020</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D167" s="2" t="s">
         <v>54</v>
       </c>
       <c r="E167" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F167" s="7" t="s">
         <v>6</v>
@@ -6645,7 +6679,7 @@
         <v>2020</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C168" s="2"/>
       <c r="D168" s="2" t="s">
@@ -6670,16 +6704,16 @@
         <v>2020</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D169" s="2" t="s">
         <v>54</v>
       </c>
       <c r="E169" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F169" s="7" t="s">
         <v>6</v>
@@ -6697,16 +6731,16 @@
         <v>2020</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D170" s="2" t="s">
         <v>144</v>
       </c>
       <c r="E170" s="2" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="F170" s="7" t="s">
         <v>6</v>
@@ -6724,16 +6758,16 @@
         <v>2020</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D171" s="2" t="s">
         <v>54</v>
       </c>
       <c r="E171" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F171" s="7" t="s">
         <v>6</v>
@@ -6751,10 +6785,10 @@
         <v>2020</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D172" s="2" t="s">
         <v>54</v>
@@ -6778,14 +6812,14 @@
         <v>2020</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C173" s="2"/>
       <c r="D173" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E173" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F173" s="7" t="s">
         <v>6</v>
@@ -6803,16 +6837,16 @@
         <v>2020</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D174" s="2" t="s">
         <v>141</v>
       </c>
       <c r="E174" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F174" s="7" t="s">
         <v>6</v>
@@ -6830,16 +6864,16 @@
         <v>2020</v>
       </c>
       <c r="B175" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="C175" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="D175" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="E175" s="2" t="s">
         <v>315</v>
-      </c>
-      <c r="C175" s="2" t="s">
-        <v>444</v>
-      </c>
-      <c r="D175" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="E175" s="2" t="s">
-        <v>316</v>
       </c>
       <c r="F175" s="7" t="s">
         <v>6</v>
@@ -6857,16 +6891,16 @@
         <v>2021</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D176" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E176" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F176" s="7" t="s">
         <v>6</v>
@@ -6884,16 +6918,16 @@
         <v>2021</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D177" s="2" t="s">
         <v>54</v>
       </c>
       <c r="E177" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F177" s="7" t="s">
         <v>6</v>
@@ -6911,16 +6945,16 @@
         <v>2021</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D178" s="2" t="s">
         <v>141</v>
       </c>
       <c r="E178" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F178" s="7" t="s">
         <v>6</v>
@@ -6938,16 +6972,16 @@
         <v>2021</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D179" s="2" t="s">
         <v>109</v>
       </c>
       <c r="E179" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F179" s="7" t="s">
         <v>6</v>
@@ -6965,14 +6999,14 @@
         <v>2021</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C180" s="2"/>
       <c r="D180" s="2" t="s">
         <v>216</v>
       </c>
       <c r="E180" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F180" s="7" t="s">
         <v>6</v>
@@ -6990,16 +7024,16 @@
         <v>2021</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D181" s="2" t="s">
         <v>54</v>
       </c>
       <c r="E181" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F181" s="7" t="s">
         <v>6</v>
@@ -7017,7 +7051,7 @@
         <v>2021</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C182" s="2"/>
       <c r="D182" s="2" t="s">
@@ -7042,14 +7076,14 @@
         <v>2021</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C183" s="2"/>
       <c r="D183" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E183" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F183" s="7" t="s">
         <v>6</v>
@@ -7067,7 +7101,7 @@
         <v>2021</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C184" s="2"/>
       <c r="D184" s="2" t="s">
@@ -7092,16 +7126,16 @@
         <v>2021</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D185" s="2" t="s">
         <v>54</v>
       </c>
       <c r="E185" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F185" s="7" t="s">
         <v>6</v>
@@ -7119,7 +7153,7 @@
         <v>2021</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C186" s="2"/>
       <c r="D186" s="2" t="s">
@@ -7144,16 +7178,16 @@
         <v>2021</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D187" s="2" t="s">
         <v>141</v>
       </c>
       <c r="E187" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="F187" s="7" t="s">
         <v>6</v>
@@ -7171,16 +7205,16 @@
         <v>2021</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D188" s="2" t="s">
         <v>54</v>
       </c>
       <c r="E188" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F188" s="7" t="s">
         <v>6</v>
@@ -7198,14 +7232,14 @@
         <v>2021</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C189" s="2"/>
       <c r="D189" s="2" t="s">
         <v>144</v>
       </c>
       <c r="E189" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F189" s="7" t="s">
         <v>6</v>
@@ -7226,7 +7260,7 @@
         <v>138</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D190" s="2" t="s">
         <v>30</v>
@@ -7250,16 +7284,16 @@
         <v>2021</v>
       </c>
       <c r="B191" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="C191" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="D191" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="C191" s="2" t="s">
-        <v>435</v>
-      </c>
-      <c r="D191" s="2" t="s">
+      <c r="E191" s="2" t="s">
         <v>343</v>
-      </c>
-      <c r="E191" s="2" t="s">
-        <v>344</v>
       </c>
       <c r="F191" s="7" t="s">
         <v>6</v>
@@ -7277,16 +7311,16 @@
         <v>2018</v>
       </c>
       <c r="B192" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C192" s="2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D192" s="2" t="s">
         <v>54</v>
       </c>
       <c r="E192" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F192" s="7" t="s">
         <v>6</v>
@@ -7304,16 +7338,16 @@
         <v>2022</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D193" s="2" t="s">
         <v>141</v>
       </c>
       <c r="E193" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="F193" s="7" t="s">
         <v>6</v>
@@ -7331,14 +7365,14 @@
         <v>2022</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C194" s="2"/>
       <c r="D194" s="2" t="s">
         <v>216</v>
       </c>
       <c r="E194" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F194" s="7" t="s">
         <v>6</v>
@@ -7356,16 +7390,16 @@
         <v>2022</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D195" s="2" t="s">
         <v>54</v>
       </c>
       <c r="E195" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F195" s="7" t="s">
         <v>6</v>
@@ -7383,16 +7417,16 @@
         <v>2022</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C196" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D196" s="2" t="s">
         <v>144</v>
       </c>
       <c r="E196" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F196" s="7" t="s">
         <v>6</v>
@@ -7410,14 +7444,14 @@
         <v>2022</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C197" s="2"/>
       <c r="D197" s="2" t="s">
         <v>160</v>
       </c>
       <c r="E197" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F197" s="7" t="s">
         <v>6</v>
@@ -7435,14 +7469,14 @@
         <v>2022</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C198" s="2"/>
       <c r="D198" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="E198" s="2" t="s">
         <v>362</v>
-      </c>
-      <c r="E198" s="2" t="s">
-        <v>363</v>
       </c>
       <c r="F198" s="7" t="s">
         <v>6</v>
@@ -7460,14 +7494,14 @@
         <v>2022</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="C199" s="2"/>
       <c r="D199" s="2" t="s">
         <v>109</v>
       </c>
       <c r="E199" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F199" s="7" t="s">
         <v>6</v>
@@ -7485,16 +7519,16 @@
         <v>2022</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D200" s="2" t="s">
         <v>141</v>
       </c>
       <c r="E200" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F200" s="7" t="s">
         <v>6</v>
@@ -7512,16 +7546,16 @@
         <v>2022</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C201" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D201" s="2" t="s">
         <v>154</v>
       </c>
       <c r="E201" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F201" s="7" t="s">
         <v>6</v>
@@ -7539,16 +7573,16 @@
         <v>2022</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C202" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D202" s="2" t="s">
         <v>160</v>
       </c>
       <c r="E202" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F202" s="7" t="s">
         <v>6</v>
@@ -7566,14 +7600,14 @@
         <v>2022</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C203" s="2"/>
       <c r="D203" s="2" t="s">
         <v>160</v>
       </c>
       <c r="E203" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F203" s="7" t="s">
         <v>6</v>
@@ -7591,7 +7625,7 @@
         <v>2022</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C204" s="2"/>
       <c r="D204" s="2" t="s">
@@ -7616,16 +7650,16 @@
         <v>2023</v>
       </c>
       <c r="B205" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C205" s="2" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D205" s="2" t="s">
         <v>54</v>
       </c>
       <c r="E205" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F205" s="7" t="s">
         <v>6</v>
@@ -7643,10 +7677,10 @@
         <v>2023</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C206" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D206" s="2" t="s">
         <v>25</v>
@@ -7670,14 +7704,14 @@
         <v>2023</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C207" s="2"/>
       <c r="D207" s="2" t="s">
         <v>160</v>
       </c>
       <c r="E207" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F207" s="7" t="s">
         <v>6</v>
@@ -7695,14 +7729,14 @@
         <v>2023</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C208" s="2"/>
       <c r="D208" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="E208" s="2" t="s">
         <v>370</v>
-      </c>
-      <c r="E208" s="2" t="s">
-        <v>371</v>
       </c>
       <c r="F208" s="7" t="s">
         <v>6</v>
@@ -7720,14 +7754,14 @@
         <v>2023</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C209" s="2"/>
       <c r="D209" s="2" t="s">
         <v>160</v>
       </c>
       <c r="E209" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F209" s="7" t="s">
         <v>6</v>
@@ -7745,7 +7779,7 @@
         <v>2023</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C210" s="2"/>
       <c r="D210" s="2" t="s">
@@ -7770,14 +7804,14 @@
         <v>2023</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C211" s="2"/>
       <c r="D211" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E211" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F211" s="7" t="s">
         <v>6</v>
@@ -7795,7 +7829,7 @@
         <v>2023</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C212" s="2"/>
       <c r="D212" s="2" t="s">
@@ -7820,16 +7854,16 @@
         <v>2023</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C213" s="2" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D213" s="2" t="s">
         <v>141</v>
       </c>
       <c r="E213" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F213" s="7" t="s">
         <v>6</v>
@@ -7872,7 +7906,7 @@
         <v>2023</v>
       </c>
       <c r="B215" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C215" s="2"/>
       <c r="D215" s="2" t="s">
@@ -7897,14 +7931,14 @@
         <v>2023</v>
       </c>
       <c r="B216" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C216" s="2"/>
       <c r="D216" s="2" t="s">
         <v>160</v>
       </c>
       <c r="E216" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F216" s="7" t="s">
         <v>6</v>
@@ -7922,14 +7956,14 @@
         <v>2023</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C217" s="2"/>
       <c r="D217" s="2" t="s">
         <v>109</v>
       </c>
       <c r="E217" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F217" s="7" t="s">
         <v>6</v>
@@ -7947,14 +7981,14 @@
         <v>2023</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C218" s="2"/>
       <c r="D218" s="2" t="s">
         <v>141</v>
       </c>
       <c r="E218" s="2" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F218" s="7" t="s">
         <v>6</v>
@@ -7972,13 +8006,13 @@
         <v>2024</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D219" s="2" t="s">
         <v>35</v>
       </c>
       <c r="E219" s="2" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F219" s="7" t="s">
         <v>6</v>
@@ -7995,14 +8029,14 @@
         <v>2024</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>464</v>
-      </c>
-      <c r="C220" s="14"/>
+        <v>463</v>
+      </c>
+      <c r="C220" s="13"/>
       <c r="D220" s="2" t="s">
         <v>35</v>
       </c>
       <c r="E220" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F220" s="7" t="s">
         <v>6</v>
@@ -8019,16 +8053,16 @@
         <v>2024</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C221" s="2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D221" s="2" t="s">
         <v>54</v>
       </c>
       <c r="E221" s="2" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="F221" s="7" t="s">
         <v>6</v>
@@ -8045,14 +8079,14 @@
         <v>2024</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C222" s="2"/>
       <c r="D222" s="2" t="s">
         <v>160</v>
       </c>
       <c r="E222" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="F222" s="7" t="s">
         <v>6</v>
@@ -8069,14 +8103,14 @@
         <v>2024</v>
       </c>
       <c r="B223" s="2" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C223" s="2"/>
       <c r="D223" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="E223" s="2" t="s">
         <v>468</v>
-      </c>
-      <c r="E223" s="2" t="s">
-        <v>469</v>
       </c>
       <c r="F223" s="7" t="s">
         <v>6</v>
@@ -8093,16 +8127,16 @@
         <v>2024</v>
       </c>
       <c r="B224" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="C224" s="2" t="s">
         <v>471</v>
       </c>
-      <c r="C224" s="2" t="s">
+      <c r="D224" s="2" t="s">
         <v>472</v>
       </c>
-      <c r="D224" s="2" t="s">
+      <c r="E224" s="2" t="s">
         <v>473</v>
-      </c>
-      <c r="E224" s="2" t="s">
-        <v>474</v>
       </c>
       <c r="F224" s="2" t="s">
         <v>6</v>
@@ -8119,16 +8153,16 @@
         <v>2024</v>
       </c>
       <c r="B225" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C225" s="2" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D225" s="2" t="s">
         <v>141</v>
       </c>
       <c r="E225" s="2" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="F225" s="2" t="s">
         <v>6</v>
@@ -8145,16 +8179,16 @@
         <v>2024</v>
       </c>
       <c r="B226" s="2" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C226" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D226" s="2" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="E226" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="F226" s="7" t="s">
         <v>6</v>
@@ -8172,16 +8206,16 @@
         <v>2024</v>
       </c>
       <c r="B227" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="C227" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="D227" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="E227" s="2" t="s">
         <v>484</v>
-      </c>
-      <c r="C227" s="2" t="s">
-        <v>489</v>
-      </c>
-      <c r="D227" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="E227" s="2" t="s">
-        <v>485</v>
       </c>
       <c r="F227" s="7" t="s">
         <v>6</v>
@@ -8198,16 +8232,16 @@
         <v>2024</v>
       </c>
       <c r="B228" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="C228" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="D228" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="E228" s="2" t="s">
         <v>480</v>
-      </c>
-      <c r="C228" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="D228" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="E228" s="2" t="s">
-        <v>481</v>
       </c>
       <c r="F228" s="7" t="s">
         <v>6</v>
@@ -8224,16 +8258,16 @@
         <v>2024</v>
       </c>
       <c r="B229" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C229" s="2" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D229" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E229" s="2" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="F229" s="7" t="s">
         <v>6</v>
@@ -8250,14 +8284,14 @@
         <v>2024</v>
       </c>
       <c r="B230" s="2" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C230" s="2"/>
       <c r="D230" s="2" t="s">
         <v>216</v>
       </c>
       <c r="E230" s="2" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="F230" s="7" t="s">
         <v>6</v>
@@ -8274,16 +8308,16 @@
         <v>2024</v>
       </c>
       <c r="B231" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="C231" s="2" t="s">
         <v>497</v>
-      </c>
-      <c r="C231" s="2" t="s">
-        <v>498</v>
       </c>
       <c r="D231" s="2" t="s">
         <v>141</v>
       </c>
       <c r="E231" s="2" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="F231" s="7" t="s">
         <v>6</v>
@@ -8300,10 +8334,10 @@
         <v>2024</v>
       </c>
       <c r="B232" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C232" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D232" s="2" t="s">
         <v>38</v>
@@ -8326,16 +8360,16 @@
         <v>2024</v>
       </c>
       <c r="B233" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="C233" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="C233" s="2" t="s">
-        <v>501</v>
-      </c>
-      <c r="D233" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E233" s="2" t="s">
-        <v>504</v>
+      <c r="D233" s="14" t="s">
+        <v>532</v>
+      </c>
+      <c r="E233" s="14" t="s">
+        <v>533</v>
       </c>
       <c r="F233" s="7" t="s">
         <v>6</v>
@@ -8352,13 +8386,13 @@
         <v>2024</v>
       </c>
       <c r="B234" s="2" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D234" s="2" t="s">
         <v>109</v>
       </c>
       <c r="E234" s="2" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="F234" s="7" t="s">
         <v>6</v>
@@ -8375,10 +8409,10 @@
         <v>2024</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C235" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D235" s="2" t="s">
         <v>30</v>
@@ -8401,208 +8435,311 @@
         <v>2025</v>
       </c>
       <c r="B236" s="2" t="s">
+        <v>512</v>
+      </c>
+      <c r="C236" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="D236" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="E236" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="F236" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G236" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H236" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="237" spans="1:9" ht="29" x14ac:dyDescent="0.2">
+      <c r="A237" s="5">
+        <v>2025</v>
+      </c>
+      <c r="B237" s="14" t="s">
+        <v>513</v>
+      </c>
+      <c r="C237" s="14" t="s">
+        <v>530</v>
+      </c>
+      <c r="D237" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="E237" s="14" t="s">
+        <v>518</v>
+      </c>
+      <c r="F237" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G237" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H237" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="238" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A238" s="5">
+        <v>2025</v>
+      </c>
+      <c r="B238" s="14" t="s">
         <v>514</v>
       </c>
-      <c r="C236" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="D236" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="E236" s="2" t="s">
-        <v>481</v>
-      </c>
-      <c r="F236" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G236" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="H236" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="237" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A237" s="7">
+      <c r="C238" s="14" t="s">
+        <v>412</v>
+      </c>
+      <c r="D238" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E238" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="F238" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G238" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H238" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="239" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A239" s="5">
         <v>2025</v>
       </c>
-      <c r="B237" s="2" t="s">
-        <v>515</v>
-      </c>
-      <c r="C237" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="D237" s="2" t="s">
+      <c r="B239" s="14" t="s">
+        <v>516</v>
+      </c>
+      <c r="C239" s="12"/>
+      <c r="D239" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E239" s="14" t="s">
+        <v>517</v>
+      </c>
+      <c r="F239" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G239" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H239" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="240" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A240" s="5">
+        <v>2025</v>
+      </c>
+      <c r="B240" s="14" t="s">
+        <v>527</v>
+      </c>
+      <c r="C240" s="12"/>
+      <c r="D240" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="E240" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="F240" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G240" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H240" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="241" spans="1:9" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.2">
+      <c r="A241" s="5">
+        <v>2025</v>
+      </c>
+      <c r="B241" s="14" t="s">
+        <v>520</v>
+      </c>
+      <c r="C241" s="14" t="s">
+        <v>522</v>
+      </c>
+      <c r="D241" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="E241" s="14" t="s">
+        <v>521</v>
+      </c>
+      <c r="F241" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G241" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H241" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="242" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A242" s="5">
+        <v>2025</v>
+      </c>
+      <c r="B242" s="14" t="s">
+        <v>529</v>
+      </c>
+      <c r="C242" s="14" t="s">
+        <v>528</v>
+      </c>
+      <c r="D242" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="E237" s="2" t="s">
-        <v>520</v>
-      </c>
-      <c r="F237" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G237" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="H237" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="238" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A238" s="7">
+      <c r="E242" s="14" t="s">
+        <v>523</v>
+      </c>
+      <c r="F242" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G242" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H242" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="243" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A243" s="5">
         <v>2025</v>
       </c>
-      <c r="B238" s="2" t="s">
-        <v>516</v>
-      </c>
-      <c r="C238" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D238" s="2" t="s">
+      <c r="B243" s="14" t="s">
+        <v>524</v>
+      </c>
+      <c r="C243" s="14" t="s">
+        <v>526</v>
+      </c>
+      <c r="D243" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E238" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="F238" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G238" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="H238" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="239" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A239" s="7">
+      <c r="E243" s="14" t="s">
+        <v>525</v>
+      </c>
+      <c r="F243" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G243" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H243" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="244" spans="1:9" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A244" s="5">
         <v>2025</v>
       </c>
-      <c r="B239" s="2" t="s">
-        <v>518</v>
-      </c>
-      <c r="D239" s="2" t="s">
+      <c r="B244" s="14" t="s">
+        <v>531</v>
+      </c>
+      <c r="C244" s="14"/>
+      <c r="D244" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="E244" s="14" t="s">
+        <v>354</v>
+      </c>
+      <c r="F244" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G244" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H244" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="245" spans="1:9" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A245" s="5">
+        <v>2025</v>
+      </c>
+      <c r="B245" s="5" t="s">
+        <v>534</v>
+      </c>
+      <c r="C245" s="5" t="s">
+        <v>389</v>
+      </c>
+      <c r="D245" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E239" s="2" t="s">
-        <v>519</v>
-      </c>
-      <c r="F239" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G239" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="H239" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="240" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A240" s="7">
+      <c r="E245" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F245" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G245" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H245" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="246" spans="1:9" ht="43" x14ac:dyDescent="0.2">
+      <c r="A246" s="5">
         <v>2025</v>
       </c>
-      <c r="B240" s="10" t="s">
-        <v>529</v>
-      </c>
-      <c r="C240" s="12"/>
-      <c r="D240" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="E240" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="F240" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G240" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="H240" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="241" spans="1:8" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.2">
-      <c r="A241" s="4">
+      <c r="B246" s="5" t="s">
+        <v>535</v>
+      </c>
+      <c r="C246" s="14" t="s">
+        <v>537</v>
+      </c>
+      <c r="D246" s="5" t="s">
+        <v>536</v>
+      </c>
+      <c r="E246" s="5" t="s">
+        <v>538</v>
+      </c>
+      <c r="F246" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G246" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H246" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I246" s="6"/>
+    </row>
+    <row r="247" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A247" s="5">
         <v>2025</v>
       </c>
-      <c r="B241" s="10" t="s">
-        <v>522</v>
-      </c>
-      <c r="C241" s="10" t="s">
-        <v>524</v>
-      </c>
-      <c r="D241" s="10" t="s">
-        <v>165</v>
-      </c>
-      <c r="E241" s="10" t="s">
-        <v>523</v>
-      </c>
-      <c r="F241" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G241" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H241" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="242" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A242" s="4">
-        <v>2025</v>
-      </c>
-      <c r="B242" s="10" t="s">
-        <v>531</v>
-      </c>
-      <c r="C242" s="10" t="s">
-        <v>530</v>
-      </c>
-      <c r="D242" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="E242" s="10" t="s">
-        <v>525</v>
-      </c>
-      <c r="F242" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G242" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H242" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="243" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A243" s="4">
-        <v>2025</v>
-      </c>
-      <c r="B243" s="10" t="s">
-        <v>526</v>
-      </c>
-      <c r="C243" s="10" t="s">
-        <v>528</v>
-      </c>
-      <c r="D243" s="10" t="s">
+      <c r="B247" s="5" t="s">
+        <v>539</v>
+      </c>
+      <c r="C247" s="5" t="s">
+        <v>540</v>
+      </c>
+      <c r="D247" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E243" s="10" t="s">
-        <v>527</v>
-      </c>
-      <c r="F243" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G243" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H243" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="244" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E244" s="2"/>
+      <c r="E247" s="5" t="s">
+        <v>541</v>
+      </c>
+      <c r="F247" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G247" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H247" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I247" s="6"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I247" xr:uid="{6B89377A-76F6-CA40-8081-AAD80BFAB6B8}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H217">
     <sortCondition ref="B2:B217"/>
   </sortState>
@@ -8626,37 +8763,37 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="59" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="45" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add oncology tx updates
</commit_message>
<xml_diff>
--- a/src/main/webapp/content/files/oncologyTherapies/fda_approved_oncology_therapies.xlsx
+++ b/src/main/webapp/content/files/oncologyTherapies/fda_approved_oncology_therapies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cavendk1/Documents/New onc therapies/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luc2/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59E48DA2-5F66-174E-9D87-A0BE250055A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1B02D45-5751-7242-90DF-9362D1C95D5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3480" yWindow="-21100" windowWidth="30240" windowHeight="17460" xr2:uid="{D862B214-800F-AF40-9BAA-60FE1781D5C8}"/>
+    <workbookView xWindow="7560" yWindow="2100" windowWidth="35060" windowHeight="20900" xr2:uid="{D862B214-800F-AF40-9BAA-60FE1781D5C8}"/>
   </bookViews>
   <sheets>
     <sheet name="FDA-Approved Oncology Therapies" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'FDA-Approved Oncology Therapies'!$A$1:$I$247</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1622" uniqueCount="543">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1636" uniqueCount="547">
   <si>
     <t>Year of drug’s first FDA- approval</t>
   </si>
@@ -1686,9 +1686,6 @@
     <t>Revumenib</t>
   </si>
   <si>
-    <t>KMT2A Rearrangement</t>
-  </si>
-  <si>
     <t>Zanidatamab</t>
   </si>
   <si>
@@ -1879,6 +1876,22 @@
   </si>
   <si>
     <t>EGFR/HER2 (ERBB2)/HER4 (ERBB4) inhibitor</t>
+  </si>
+  <si>
+    <t>Imlunestrant</t>
+  </si>
+  <si>
+    <t>Ziftomenib</t>
+  </si>
+  <si>
+    <t>Susceptible NPM1 mutations, which includes W288Cfs*12 and W290Rfs*10</t>
+  </si>
+  <si>
+    <t>*KMT2A Rearrangement
+*Susceptible NPM1 mutations, which includes W288Cfs*12 and W290Rfs*10</t>
+  </si>
+  <si>
+    <t>ESR1 V422del, S463F, S463P, L469V, L536, Y537, D538, or E380  and ER+/HER2-</t>
   </si>
 </sst>
 </file>
@@ -1994,7 +2007,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2026,6 +2039,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2340,11 +2357,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B89377A-76F6-CA40-8081-AAD80BFAB6B8}">
-  <dimension ref="A1:I247"/>
+  <dimension ref="A1:I249"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A230" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C245" sqref="C245"/>
+      <pane ySplit="1" topLeftCell="A227" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D237" sqref="D237"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2362,16 +2379,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>503</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>504</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="8" t="s">
         <v>505</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>506</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>507</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>1</v>
@@ -3723,7 +3740,7 @@
         <v>2011</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>395</v>
@@ -4608,7 +4625,7 @@
         <v>175</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>141</v>
@@ -5128,7 +5145,7 @@
         <v>109</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F108" s="7" t="s">
         <v>6</v>
@@ -5405,7 +5422,7 @@
         <v>223</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D119" s="2" t="s">
         <v>109</v>
@@ -5519,7 +5536,7 @@
         <v>54</v>
       </c>
       <c r="E123" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="F123" s="7" t="s">
         <v>6</v>
@@ -6291,7 +6308,7 @@
         <v>269</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D153" s="2" t="s">
         <v>144</v>
@@ -6740,7 +6757,7 @@
         <v>144</v>
       </c>
       <c r="E170" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="F170" s="7" t="s">
         <v>6</v>
@@ -7494,7 +7511,7 @@
         <v>2022</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C199" s="2"/>
       <c r="D199" s="2" t="s">
@@ -8303,7 +8320,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="231" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:9" ht="57" x14ac:dyDescent="0.2">
       <c r="A231" s="7">
         <v>2024</v>
       </c>
@@ -8311,13 +8328,13 @@
         <v>496</v>
       </c>
       <c r="C231" s="2" t="s">
-        <v>497</v>
+        <v>545</v>
       </c>
       <c r="D231" s="2" t="s">
         <v>141</v>
       </c>
       <c r="E231" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="F231" s="7" t="s">
         <v>6</v>
@@ -8334,7 +8351,7 @@
         <v>2024</v>
       </c>
       <c r="B232" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C232" s="2" t="s">
         <v>434</v>
@@ -8360,16 +8377,16 @@
         <v>2024</v>
       </c>
       <c r="B233" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="C233" s="2" t="s">
         <v>499</v>
       </c>
-      <c r="C233" s="2" t="s">
-        <v>500</v>
-      </c>
       <c r="D233" s="14" t="s">
+        <v>531</v>
+      </c>
+      <c r="E233" s="14" t="s">
         <v>532</v>
-      </c>
-      <c r="E233" s="14" t="s">
-        <v>533</v>
       </c>
       <c r="F233" s="7" t="s">
         <v>6</v>
@@ -8386,13 +8403,13 @@
         <v>2024</v>
       </c>
       <c r="B234" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D234" s="2" t="s">
         <v>109</v>
       </c>
       <c r="E234" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F234" s="7" t="s">
         <v>6</v>
@@ -8409,7 +8426,7 @@
         <v>2024</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C235" s="2" t="s">
         <v>387</v>
@@ -8435,7 +8452,7 @@
         <v>2025</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C236" s="2" t="s">
         <v>413</v>
@@ -8461,16 +8478,16 @@
         <v>2025</v>
       </c>
       <c r="B237" s="14" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C237" s="14" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D237" s="14" t="s">
         <v>144</v>
       </c>
       <c r="E237" s="14" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="F237" s="5" t="s">
         <v>6</v>
@@ -8487,7 +8504,7 @@
         <v>2025</v>
       </c>
       <c r="B238" s="14" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C238" s="14" t="s">
         <v>412</v>
@@ -8513,14 +8530,14 @@
         <v>2025</v>
       </c>
       <c r="B239" s="14" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C239" s="12"/>
       <c r="D239" s="14" t="s">
         <v>54</v>
       </c>
       <c r="E239" s="14" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="F239" s="5" t="s">
         <v>6</v>
@@ -8537,7 +8554,7 @@
         <v>2025</v>
       </c>
       <c r="B240" s="14" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C240" s="12"/>
       <c r="D240" s="14" t="s">
@@ -8561,16 +8578,16 @@
         <v>2025</v>
       </c>
       <c r="B241" s="14" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C241" s="14" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D241" s="14" t="s">
         <v>165</v>
       </c>
       <c r="E241" s="14" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F241" s="5" t="s">
         <v>6</v>
@@ -8587,16 +8604,16 @@
         <v>2025</v>
       </c>
       <c r="B242" s="14" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C242" s="14" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D242" s="14" t="s">
         <v>144</v>
       </c>
       <c r="E242" s="14" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F242" s="5" t="s">
         <v>6</v>
@@ -8613,16 +8630,16 @@
         <v>2025</v>
       </c>
       <c r="B243" s="14" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C243" s="14" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D243" s="14" t="s">
         <v>54</v>
       </c>
       <c r="E243" s="14" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="F243" s="5" t="s">
         <v>6</v>
@@ -8639,7 +8656,7 @@
         <v>2025</v>
       </c>
       <c r="B244" s="14" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C244" s="14"/>
       <c r="D244" s="14" t="s">
@@ -8663,7 +8680,7 @@
         <v>2025</v>
       </c>
       <c r="B245" s="5" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C245" s="5" t="s">
         <v>389</v>
@@ -8689,16 +8706,16 @@
         <v>2025</v>
       </c>
       <c r="B246" s="5" t="s">
+        <v>534</v>
+      </c>
+      <c r="C246" s="14" t="s">
+        <v>536</v>
+      </c>
+      <c r="D246" s="5" t="s">
         <v>535</v>
       </c>
-      <c r="C246" s="14" t="s">
+      <c r="E246" s="5" t="s">
         <v>537</v>
-      </c>
-      <c r="D246" s="5" t="s">
-        <v>536</v>
-      </c>
-      <c r="E246" s="5" t="s">
-        <v>538</v>
       </c>
       <c r="F246" s="5" t="s">
         <v>6</v>
@@ -8716,16 +8733,16 @@
         <v>2025</v>
       </c>
       <c r="B247" s="5" t="s">
+        <v>538</v>
+      </c>
+      <c r="C247" s="5" t="s">
         <v>539</v>
-      </c>
-      <c r="C247" s="5" t="s">
-        <v>540</v>
       </c>
       <c r="D247" s="5" t="s">
         <v>54</v>
       </c>
       <c r="E247" s="5" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="F247" s="5" t="s">
         <v>6</v>
@@ -8737,6 +8754,58 @@
         <v>6</v>
       </c>
       <c r="I247" s="6"/>
+    </row>
+    <row r="248" spans="1:9" s="9" customFormat="1" ht="43" x14ac:dyDescent="0.2">
+      <c r="A248" s="7">
+        <v>2025</v>
+      </c>
+      <c r="B248" s="7" t="s">
+        <v>542</v>
+      </c>
+      <c r="C248" s="2" t="s">
+        <v>546</v>
+      </c>
+      <c r="D248" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E248" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F248" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G248" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H248" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="249" spans="1:9" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A249" s="7">
+        <v>2025</v>
+      </c>
+      <c r="B249" s="15" t="s">
+        <v>543</v>
+      </c>
+      <c r="C249" s="13" t="s">
+        <v>544</v>
+      </c>
+      <c r="D249" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E249" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="F249" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G249" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H249" s="16" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:I247" xr:uid="{6B89377A-76F6-CA40-8081-AAD80BFAB6B8}"/>

</xml_diff>

<commit_message>
Add oncology tx updates (#1267)
</commit_message>
<xml_diff>
--- a/src/main/webapp/content/files/oncologyTherapies/fda_approved_oncology_therapies.xlsx
+++ b/src/main/webapp/content/files/oncologyTherapies/fda_approved_oncology_therapies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cavendk1/Documents/New onc therapies/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luc2/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59E48DA2-5F66-174E-9D87-A0BE250055A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1B02D45-5751-7242-90DF-9362D1C95D5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3480" yWindow="-21100" windowWidth="30240" windowHeight="17460" xr2:uid="{D862B214-800F-AF40-9BAA-60FE1781D5C8}"/>
+    <workbookView xWindow="7560" yWindow="2100" windowWidth="35060" windowHeight="20900" xr2:uid="{D862B214-800F-AF40-9BAA-60FE1781D5C8}"/>
   </bookViews>
   <sheets>
     <sheet name="FDA-Approved Oncology Therapies" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'FDA-Approved Oncology Therapies'!$A$1:$I$247</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1622" uniqueCount="543">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1636" uniqueCount="547">
   <si>
     <t>Year of drug’s first FDA- approval</t>
   </si>
@@ -1686,9 +1686,6 @@
     <t>Revumenib</t>
   </si>
   <si>
-    <t>KMT2A Rearrangement</t>
-  </si>
-  <si>
     <t>Zanidatamab</t>
   </si>
   <si>
@@ -1879,6 +1876,22 @@
   </si>
   <si>
     <t>EGFR/HER2 (ERBB2)/HER4 (ERBB4) inhibitor</t>
+  </si>
+  <si>
+    <t>Imlunestrant</t>
+  </si>
+  <si>
+    <t>Ziftomenib</t>
+  </si>
+  <si>
+    <t>Susceptible NPM1 mutations, which includes W288Cfs*12 and W290Rfs*10</t>
+  </si>
+  <si>
+    <t>*KMT2A Rearrangement
+*Susceptible NPM1 mutations, which includes W288Cfs*12 and W290Rfs*10</t>
+  </si>
+  <si>
+    <t>ESR1 V422del, S463F, S463P, L469V, L536, Y537, D538, or E380  and ER+/HER2-</t>
   </si>
 </sst>
 </file>
@@ -1994,7 +2007,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2026,6 +2039,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2340,11 +2357,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B89377A-76F6-CA40-8081-AAD80BFAB6B8}">
-  <dimension ref="A1:I247"/>
+  <dimension ref="A1:I249"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A230" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C245" sqref="C245"/>
+      <pane ySplit="1" topLeftCell="A227" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D237" sqref="D237"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2362,16 +2379,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>503</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>504</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="8" t="s">
         <v>505</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>506</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>507</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>1</v>
@@ -3723,7 +3740,7 @@
         <v>2011</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>395</v>
@@ -4608,7 +4625,7 @@
         <v>175</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>141</v>
@@ -5128,7 +5145,7 @@
         <v>109</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F108" s="7" t="s">
         <v>6</v>
@@ -5405,7 +5422,7 @@
         <v>223</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D119" s="2" t="s">
         <v>109</v>
@@ -5519,7 +5536,7 @@
         <v>54</v>
       </c>
       <c r="E123" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="F123" s="7" t="s">
         <v>6</v>
@@ -6291,7 +6308,7 @@
         <v>269</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D153" s="2" t="s">
         <v>144</v>
@@ -6740,7 +6757,7 @@
         <v>144</v>
       </c>
       <c r="E170" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="F170" s="7" t="s">
         <v>6</v>
@@ -7494,7 +7511,7 @@
         <v>2022</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C199" s="2"/>
       <c r="D199" s="2" t="s">
@@ -8303,7 +8320,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="231" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:9" ht="57" x14ac:dyDescent="0.2">
       <c r="A231" s="7">
         <v>2024</v>
       </c>
@@ -8311,13 +8328,13 @@
         <v>496</v>
       </c>
       <c r="C231" s="2" t="s">
-        <v>497</v>
+        <v>545</v>
       </c>
       <c r="D231" s="2" t="s">
         <v>141</v>
       </c>
       <c r="E231" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="F231" s="7" t="s">
         <v>6</v>
@@ -8334,7 +8351,7 @@
         <v>2024</v>
       </c>
       <c r="B232" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C232" s="2" t="s">
         <v>434</v>
@@ -8360,16 +8377,16 @@
         <v>2024</v>
       </c>
       <c r="B233" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="C233" s="2" t="s">
         <v>499</v>
       </c>
-      <c r="C233" s="2" t="s">
-        <v>500</v>
-      </c>
       <c r="D233" s="14" t="s">
+        <v>531</v>
+      </c>
+      <c r="E233" s="14" t="s">
         <v>532</v>
-      </c>
-      <c r="E233" s="14" t="s">
-        <v>533</v>
       </c>
       <c r="F233" s="7" t="s">
         <v>6</v>
@@ -8386,13 +8403,13 @@
         <v>2024</v>
       </c>
       <c r="B234" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D234" s="2" t="s">
         <v>109</v>
       </c>
       <c r="E234" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F234" s="7" t="s">
         <v>6</v>
@@ -8409,7 +8426,7 @@
         <v>2024</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C235" s="2" t="s">
         <v>387</v>
@@ -8435,7 +8452,7 @@
         <v>2025</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C236" s="2" t="s">
         <v>413</v>
@@ -8461,16 +8478,16 @@
         <v>2025</v>
       </c>
       <c r="B237" s="14" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C237" s="14" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D237" s="14" t="s">
         <v>144</v>
       </c>
       <c r="E237" s="14" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="F237" s="5" t="s">
         <v>6</v>
@@ -8487,7 +8504,7 @@
         <v>2025</v>
       </c>
       <c r="B238" s="14" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C238" s="14" t="s">
         <v>412</v>
@@ -8513,14 +8530,14 @@
         <v>2025</v>
       </c>
       <c r="B239" s="14" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C239" s="12"/>
       <c r="D239" s="14" t="s">
         <v>54</v>
       </c>
       <c r="E239" s="14" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="F239" s="5" t="s">
         <v>6</v>
@@ -8537,7 +8554,7 @@
         <v>2025</v>
       </c>
       <c r="B240" s="14" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C240" s="12"/>
       <c r="D240" s="14" t="s">
@@ -8561,16 +8578,16 @@
         <v>2025</v>
       </c>
       <c r="B241" s="14" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C241" s="14" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D241" s="14" t="s">
         <v>165</v>
       </c>
       <c r="E241" s="14" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F241" s="5" t="s">
         <v>6</v>
@@ -8587,16 +8604,16 @@
         <v>2025</v>
       </c>
       <c r="B242" s="14" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C242" s="14" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D242" s="14" t="s">
         <v>144</v>
       </c>
       <c r="E242" s="14" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F242" s="5" t="s">
         <v>6</v>
@@ -8613,16 +8630,16 @@
         <v>2025</v>
       </c>
       <c r="B243" s="14" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C243" s="14" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D243" s="14" t="s">
         <v>54</v>
       </c>
       <c r="E243" s="14" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="F243" s="5" t="s">
         <v>6</v>
@@ -8639,7 +8656,7 @@
         <v>2025</v>
       </c>
       <c r="B244" s="14" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C244" s="14"/>
       <c r="D244" s="14" t="s">
@@ -8663,7 +8680,7 @@
         <v>2025</v>
       </c>
       <c r="B245" s="5" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C245" s="5" t="s">
         <v>389</v>
@@ -8689,16 +8706,16 @@
         <v>2025</v>
       </c>
       <c r="B246" s="5" t="s">
+        <v>534</v>
+      </c>
+      <c r="C246" s="14" t="s">
+        <v>536</v>
+      </c>
+      <c r="D246" s="5" t="s">
         <v>535</v>
       </c>
-      <c r="C246" s="14" t="s">
+      <c r="E246" s="5" t="s">
         <v>537</v>
-      </c>
-      <c r="D246" s="5" t="s">
-        <v>536</v>
-      </c>
-      <c r="E246" s="5" t="s">
-        <v>538</v>
       </c>
       <c r="F246" s="5" t="s">
         <v>6</v>
@@ -8716,16 +8733,16 @@
         <v>2025</v>
       </c>
       <c r="B247" s="5" t="s">
+        <v>538</v>
+      </c>
+      <c r="C247" s="5" t="s">
         <v>539</v>
-      </c>
-      <c r="C247" s="5" t="s">
-        <v>540</v>
       </c>
       <c r="D247" s="5" t="s">
         <v>54</v>
       </c>
       <c r="E247" s="5" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="F247" s="5" t="s">
         <v>6</v>
@@ -8737,6 +8754,58 @@
         <v>6</v>
       </c>
       <c r="I247" s="6"/>
+    </row>
+    <row r="248" spans="1:9" s="9" customFormat="1" ht="43" x14ac:dyDescent="0.2">
+      <c r="A248" s="7">
+        <v>2025</v>
+      </c>
+      <c r="B248" s="7" t="s">
+        <v>542</v>
+      </c>
+      <c r="C248" s="2" t="s">
+        <v>546</v>
+      </c>
+      <c r="D248" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E248" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F248" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G248" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H248" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="249" spans="1:9" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A249" s="7">
+        <v>2025</v>
+      </c>
+      <c r="B249" s="15" t="s">
+        <v>543</v>
+      </c>
+      <c r="C249" s="13" t="s">
+        <v>544</v>
+      </c>
+      <c r="D249" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E249" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="F249" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G249" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H249" s="16" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:I247" xr:uid="{6B89377A-76F6-CA40-8081-AAD80BFAB6B8}"/>

</xml_diff>